<commit_message>
files to tradictions English Kurdi
</commit_message>
<xml_diff>
--- a/english.xlsx
+++ b/english.xlsx
@@ -2267,7 +2267,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>الدولة</t>
+          <t>دوام كامل</t>
         </is>
       </c>
       <c r="B231" t="inlineStr"/>
@@ -2275,7 +2275,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>اسم المحافظة</t>
+          <t>دوام جزئي</t>
         </is>
       </c>
       <c r="B232" t="inlineStr"/>
@@ -2283,7 +2283,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>نوع المنظمة</t>
+          <t>استشاري</t>
         </is>
       </c>
       <c r="B233" t="inlineStr"/>
@@ -2291,7 +2291,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>شعار المنظمة</t>
+          <t>تدريب</t>
         </is>
       </c>
       <c r="B234" t="inlineStr"/>
@@ -2299,7 +2299,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>الرؤية و الرسالة</t>
+          <t>تطوع</t>
         </is>
       </c>
       <c r="B235" t="inlineStr"/>
@@ -2307,7 +2307,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>رقم الهاتف</t>
+          <t>زمالة</t>
         </is>
       </c>
       <c r="B236" t="inlineStr"/>
@@ -2315,7 +2315,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>الفئات المستهدفة</t>
+          <t>الخبرة غير ضرورية</t>
         </is>
       </c>
       <c r="B237" t="inlineStr"/>
@@ -2323,7 +2323,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>تاريخ سنة التأسيس</t>
+          <t>1-2 سنة</t>
         </is>
       </c>
       <c r="B238" t="inlineStr"/>
@@ -2331,7 +2331,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>هل المنظمة مسجلة ؟</t>
+          <t>2-5 سنة</t>
         </is>
       </c>
       <c r="B239" t="inlineStr"/>
@@ -2339,7 +2339,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>بلد التسجيل</t>
+          <t>5-9 سنة</t>
         </is>
       </c>
       <c r="B240" t="inlineStr"/>
@@ -2347,7 +2347,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>عدد اﻷعضاء</t>
+          <t>10 وفوق</t>
         </is>
       </c>
       <c r="B241" t="inlineStr"/>
@@ -2355,7 +2355,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>عدد النساء من اﻷعضاء</t>
+          <t>أقل من 6 أشهر</t>
         </is>
       </c>
       <c r="B242" t="inlineStr"/>
@@ -2363,7 +2363,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>السياسات واللوائح المكتوبة</t>
+          <t>ستة أشهر لسنة</t>
         </is>
       </c>
       <c r="B243" t="inlineStr"/>
@@ -2371,7 +2371,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>ھل المؤسسة عضو في اي شبكة او تحالف او جسم تنسیقي؟</t>
+          <t>سنة إلى سنتين</t>
         </is>
       </c>
       <c r="B244" t="inlineStr"/>
@@ -2379,7 +2379,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>عنوان الخبر</t>
+          <t>أكثر من سنتين</t>
         </is>
       </c>
       <c r="B245" t="inlineStr"/>
@@ -2387,7 +2387,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>تفاصيل الخبر</t>
+          <t>أقل من 5000 دولار</t>
         </is>
       </c>
       <c r="B246" t="inlineStr"/>
@@ -2395,7 +2395,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>صورة الخبر</t>
+          <t>بين 5000 و 10000 دولار</t>
         </is>
       </c>
       <c r="B247" t="inlineStr"/>
@@ -2403,7 +2403,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>عنوان التقرير</t>
+          <t>بين 10000 و50000 دولار</t>
         </is>
       </c>
       <c r="B248" t="inlineStr"/>
@@ -2411,7 +2411,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>مجال التقرير</t>
+          <t>بين 50000 و100000 دولار</t>
         </is>
       </c>
       <c r="B249" t="inlineStr"/>
@@ -2419,7 +2419,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>صورة او ملف التقرير</t>
+          <t>كلية</t>
         </is>
       </c>
       <c r="B250" t="inlineStr"/>
@@ -2427,7 +2427,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>عنوان البيان</t>
+          <t>جزئية</t>
         </is>
       </c>
       <c r="B251" t="inlineStr"/>
@@ -2435,7 +2435,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>صورة او ملف البيان</t>
+          <t>دراسية</t>
         </is>
       </c>
       <c r="B252" t="inlineStr"/>
@@ -2443,7 +2443,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>عنوان المحتوى</t>
+          <t>انتاجية</t>
         </is>
       </c>
       <c r="B253" t="inlineStr"/>
@@ -2451,7 +2451,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>صورة او ملف المحتوى</t>
+          <t>دراسات و أبحاث</t>
         </is>
       </c>
       <c r="B254" t="inlineStr"/>
@@ -2459,7 +2459,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>رابط المحتوى</t>
+          <t>إجازة جامعية</t>
         </is>
       </c>
       <c r="B255" t="inlineStr"/>
@@ -2467,7 +2467,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>اسم الجهة</t>
+          <t>دبلوم</t>
         </is>
       </c>
       <c r="B256" t="inlineStr"/>
@@ -2475,7 +2475,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>عنوان البحث</t>
+          <t>ماجيستير</t>
         </is>
       </c>
       <c r="B257" t="inlineStr"/>
@@ -2483,7 +2483,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>مجال البحث</t>
+          <t>دكتوراه</t>
         </is>
       </c>
       <c r="B258" t="inlineStr"/>
@@ -2491,7 +2491,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>ملف البحث</t>
+          <t>إعلام/ اتصالات/ علاقات عامة</t>
         </is>
       </c>
       <c r="B259" t="inlineStr"/>
@@ -2499,7 +2499,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>رابط البحث</t>
+          <t>أعمال وإدارة</t>
         </is>
       </c>
       <c r="B260" t="inlineStr"/>
@@ -2507,7 +2507,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>دوام كامل</t>
+          <t>اقتصاد/ محاسبة</t>
         </is>
       </c>
       <c r="B261" t="inlineStr"/>
@@ -2515,7 +2515,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>دوام جزئي</t>
+          <t>تعليم/ تربية/ رياض أطفال</t>
         </is>
       </c>
       <c r="B262" t="inlineStr"/>
@@ -2523,7 +2523,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>استشاري</t>
+          <t>حاسوب وتكنولوجيا المعلومات</t>
         </is>
       </c>
       <c r="B263" t="inlineStr"/>
@@ -2531,7 +2531,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>تدريب</t>
+          <t>دراسات إسلامية</t>
         </is>
       </c>
       <c r="B264" t="inlineStr"/>
@@ -2539,7 +2539,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>تطوع</t>
+          <t>دراسات إنسانية/ لغات</t>
         </is>
       </c>
       <c r="B265" t="inlineStr"/>
@@ -2547,7 +2547,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>زمالة</t>
+          <t>زراعة وعلوم بيئية</t>
         </is>
       </c>
       <c r="B266" t="inlineStr"/>
@@ -2555,7 +2555,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>الخبرة غير ضرورية</t>
+          <t>سياحة وعلوم فندقية</t>
         </is>
       </c>
       <c r="B267" t="inlineStr"/>
@@ -2563,7 +2563,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>1-2 سنة</t>
+          <t>علوم إنسانية</t>
         </is>
       </c>
       <c r="B268" t="inlineStr"/>
@@ -2571,7 +2571,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>2-5 سنة</t>
+          <t>علوم طبية/ طب/ صيدلة/ تمريض</t>
         </is>
       </c>
       <c r="B269" t="inlineStr"/>
@@ -2579,7 +2579,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>5-9 سنة</t>
+          <t>علوم طبيعية</t>
         </is>
       </c>
       <c r="B270" t="inlineStr"/>
@@ -2587,7 +2587,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>10 وفوق</t>
+          <t>عمارة وتصميم</t>
         </is>
       </c>
       <c r="B271" t="inlineStr"/>
@@ -2595,7 +2595,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>عنوان الوظيفة</t>
+          <t>فنون ومسارح وموسيقى</t>
         </is>
       </c>
       <c r="B272" t="inlineStr"/>
@@ -2603,7 +2603,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>مدة العقد بالأشهر</t>
+          <t>قانون ودراسات قانونية</t>
         </is>
       </c>
       <c r="B273" t="inlineStr"/>
@@ -2611,7 +2611,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>وصف الوضيفة</t>
+          <t>هندسة وعلوم هندسية</t>
         </is>
       </c>
       <c r="B274" t="inlineStr"/>
@@ -2619,7 +2619,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>المنطقة</t>
+          <t>الدولة</t>
         </is>
       </c>
       <c r="B275" t="inlineStr"/>
@@ -2627,7 +2627,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>تاريخ إغلاق الوظيفة</t>
+          <t>اسم المحافظة</t>
         </is>
       </c>
       <c r="B276" t="inlineStr"/>
@@ -2635,7 +2635,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>طريقة التقدم للوظيفة</t>
+          <t>اسم المستخدم</t>
         </is>
       </c>
       <c r="B277" t="inlineStr"/>
@@ -2643,7 +2643,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>أقل من 6 أشهر</t>
+          <t>نوع المنظمة</t>
         </is>
       </c>
       <c r="B278" t="inlineStr"/>
@@ -2651,7 +2651,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>ستة أشهر لسنة</t>
+          <t>شعار المنظمة</t>
         </is>
       </c>
       <c r="B279" t="inlineStr"/>
@@ -2659,7 +2659,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>سنة إلى سنتين</t>
+          <t>الرؤية و الرسالة</t>
         </is>
       </c>
       <c r="B280" t="inlineStr"/>
@@ -2667,7 +2667,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>أكثر من سنتين</t>
+          <t>رقم الهاتف</t>
         </is>
       </c>
       <c r="B281" t="inlineStr"/>
@@ -2675,7 +2675,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>أقل من 5000 دولار</t>
+          <t>الفئات المستهدفة</t>
         </is>
       </c>
       <c r="B282" t="inlineStr"/>
@@ -2683,7 +2683,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>بين 5000 و 10000 دولار</t>
+          <t>تاريخ سنة التأسيس</t>
         </is>
       </c>
       <c r="B283" t="inlineStr"/>
@@ -2691,7 +2691,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>بين 10000 و50000 دولار</t>
+          <t>هل المنظمة مسجلة ؟</t>
         </is>
       </c>
       <c r="B284" t="inlineStr"/>
@@ -2699,7 +2699,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>بين 50000 و100000 دولار</t>
+          <t>بلد التسجيل</t>
         </is>
       </c>
       <c r="B285" t="inlineStr"/>
@@ -2707,7 +2707,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>لمحة عن الجهة المانحة</t>
+          <t>عدد اﻷعضاء</t>
         </is>
       </c>
       <c r="B286" t="inlineStr"/>
@@ -2715,7 +2715,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>قطاع المنحة</t>
+          <t>عدد النساء من اﻷعضاء</t>
         </is>
       </c>
       <c r="B287" t="inlineStr"/>
@@ -2723,7 +2723,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>دول المنحة</t>
+          <t>السياسات واللوائح المكتوبة</t>
         </is>
       </c>
       <c r="B288" t="inlineStr"/>
@@ -2731,7 +2731,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>تاريخ إغلاق المنحة</t>
+          <t>ھل المؤسسة عضو في اي شبكة او تحالف او جسم تنسیقي؟</t>
         </is>
       </c>
       <c r="B289" t="inlineStr"/>
@@ -2739,7 +2739,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>مدة المنحة</t>
+          <t>عنوان الخبر</t>
         </is>
       </c>
       <c r="B290" t="inlineStr"/>
@@ -2747,7 +2747,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t xml:space="preserve"> حجم المنحة</t>
+          <t>تفاصيل الخبر</t>
         </is>
       </c>
       <c r="B291" t="inlineStr"/>
@@ -2755,7 +2755,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>صف المنحة</t>
+          <t>صورة الخبر</t>
         </is>
       </c>
       <c r="B292" t="inlineStr"/>
@@ -2763,7 +2763,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>شروط المنحة</t>
+          <t>عنوان التقرير</t>
         </is>
       </c>
       <c r="B293" t="inlineStr"/>
@@ -2771,7 +2771,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>متطلبات التقديم</t>
+          <t>مجال التقرير</t>
         </is>
       </c>
       <c r="B294" t="inlineStr"/>
@@ -2779,7 +2779,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>كيفية التقديم</t>
+          <t>صورة او ملف التقرير</t>
         </is>
       </c>
       <c r="B295" t="inlineStr"/>
@@ -2787,7 +2787,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>الرابط الأصلي</t>
+          <t>عنوان البيان</t>
         </is>
       </c>
       <c r="B296" t="inlineStr"/>
@@ -2795,7 +2795,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>اسم الجهة الممولة</t>
+          <t>صورة او ملف البيان</t>
         </is>
       </c>
       <c r="B297" t="inlineStr"/>
@@ -2803,7 +2803,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>عنوان الفرصة</t>
+          <t>عنوان المحتوى</t>
         </is>
       </c>
       <c r="B298" t="inlineStr"/>
@@ -2811,7 +2811,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>وصف الفرصة</t>
+          <t>صورة او ملف المحتوى</t>
         </is>
       </c>
       <c r="B299" t="inlineStr"/>
@@ -2819,7 +2819,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>نوع الفرصة</t>
+          <t>رابط المحتوى</t>
         </is>
       </c>
       <c r="B300" t="inlineStr"/>
@@ -2827,7 +2827,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>مكان الفرصة</t>
+          <t>اسم الجهة</t>
         </is>
       </c>
       <c r="B301" t="inlineStr"/>
@@ -2835,7 +2835,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>قطاع الفرصة</t>
+          <t>عنوان البحث</t>
         </is>
       </c>
       <c r="B302" t="inlineStr"/>
@@ -2843,7 +2843,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>طريقة التقديم</t>
+          <t>مجال البحث</t>
         </is>
       </c>
       <c r="B303" t="inlineStr"/>
@@ -2851,7 +2851,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>تطوير وإدارة المشاريع</t>
+          <t>ملف البحث</t>
         </is>
       </c>
       <c r="B304" t="inlineStr"/>
@@ -2859,7 +2859,7 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>الحوكمة التنظيمية</t>
+          <t>رابط البحث</t>
         </is>
       </c>
       <c r="B305" t="inlineStr"/>
@@ -2867,7 +2867,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>المناصرة والحملات</t>
+          <t>اضف اسم المنظمة اﻷخرى</t>
         </is>
       </c>
       <c r="B306" t="inlineStr"/>
@@ -2875,7 +2875,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>مكتبة المجتمع المدني</t>
+          <t>اسم المنظمة اﻷخرى</t>
         </is>
       </c>
       <c r="B307" t="inlineStr"/>
@@ -2883,7 +2883,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>تاريخ الإعداد/النشر/التأليف</t>
+          <t>عنوان الوظيفة</t>
         </is>
       </c>
       <c r="B308" t="inlineStr"/>
@@ -2891,7 +2891,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t xml:space="preserve">اسم الجهة </t>
+          <t>مدة العقد بالأشهر</t>
         </is>
       </c>
       <c r="B309" t="inlineStr"/>
@@ -2899,7 +2899,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>لمحة عن الجهة</t>
+          <t>وصف الوضيفة</t>
         </is>
       </c>
       <c r="B310" t="inlineStr"/>
@@ -2907,31 +2907,23 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t xml:space="preserve">تم إنشاء حسابك بنجاح باسم المستخدم ( {username} ) !, يرجى تأكيد عنوان بريدك الإلكتروني لإكمال التسجيل </t>
-        </is>
-      </c>
-      <c r="B311" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Your Account has been created Successful with username ( {username} ) !, Please confirm your email address to complete the registration </t>
-        </is>
-      </c>
+          <t>المنطقة</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr"/>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>يرجى التسجيل باستخدام عنوان بريد إلكتروني آخر، هذا البريد الإلكتروني ( {user_email} ) مستخدم مسبقاً</t>
-        </is>
-      </c>
-      <c r="B312" t="inlineStr">
-        <is>
-          <t>Please Sign-up with another email address, this email ( {user_email} ) is already in use</t>
-        </is>
-      </c>
+          <t>تاريخ إغلاق الوظيفة</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr"/>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>لقد تم حذف المحافظه بنجاح</t>
+          <t>طريقة التقدم للوظيفة</t>
         </is>
       </c>
       <c r="B313" t="inlineStr"/>
@@ -2939,7 +2931,7 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>لقد تم تعديل الملف الشخصي بنجاح</t>
+          <t>لوغو الجهة المانحة</t>
         </is>
       </c>
       <c r="B314" t="inlineStr"/>
@@ -2947,7 +2939,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>لقد تم حذف الملف بنجاح</t>
+          <t>لمحة عن الجهة المانحة</t>
         </is>
       </c>
       <c r="B315" t="inlineStr"/>
@@ -2955,7 +2947,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>لا يوجد حاليا منظمات</t>
+          <t>قطاع المنحة</t>
         </is>
       </c>
       <c r="B316" t="inlineStr"/>
@@ -2963,7 +2955,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>لا يوجد حالي أخبار</t>
+          <t>دول المنحة</t>
         </is>
       </c>
       <c r="B317" t="inlineStr"/>
@@ -2971,7 +2963,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>لا يوجد حاليا فرص بناء</t>
+          <t>تاريخ إغلاق المنحة</t>
         </is>
       </c>
       <c r="B318" t="inlineStr"/>
@@ -2979,7 +2971,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>لقد تم طلب الاشتراك بآخر اﻷخبار بنجاح</t>
+          <t>مدة المنحة</t>
         </is>
       </c>
       <c r="B319" t="inlineStr"/>
@@ -2987,7 +2979,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>هذا البريد الالكتروني موجود مسبقاً يرجى التسجيل ببريد الكتروني أخر</t>
+          <t>حجم المنحة</t>
         </is>
       </c>
       <c r="B320" t="inlineStr"/>
@@ -2995,7 +2987,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>لقد تم تغيير حالة الطلب للمنظمة بنجاح</t>
+          <t>وصف المنحة</t>
         </is>
       </c>
       <c r="B321" t="inlineStr"/>
@@ -3003,7 +2995,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>لقد تمت إضافة الخبر بنجاح و ستتم دراسته قريباً</t>
+          <t>شروط المنحة</t>
         </is>
       </c>
       <c r="B322" t="inlineStr"/>
@@ -3011,7 +3003,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>لقد تم تغيير حالة الخبر بنجاح</t>
+          <t>متطلبات التقديم</t>
         </is>
       </c>
       <c r="B323" t="inlineStr"/>
@@ -3019,7 +3011,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>لقد تم تعديل الخبر بنجاح</t>
+          <t>كيفية التقديم</t>
         </is>
       </c>
       <c r="B324" t="inlineStr"/>
@@ -3027,7 +3019,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>لقد تم حذف الخبر بنجاح</t>
+          <t>الرابط الأصلي</t>
         </is>
       </c>
       <c r="B325" t="inlineStr"/>
@@ -3035,7 +3027,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>لقد تمت إضافة التقرير بنجاح و ستتم دراسته قريباً</t>
+          <t>فئة المنحة</t>
         </is>
       </c>
       <c r="B326" t="inlineStr"/>
@@ -3043,7 +3035,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>لقد تم تعديل التقرير بنجاح</t>
+          <t>نوع المنحة</t>
         </is>
       </c>
       <c r="B327" t="inlineStr"/>
@@ -3051,7 +3043,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>لقد تم حذف التقرري بنجاح</t>
+          <t>المستوى التعليمي</t>
         </is>
       </c>
       <c r="B328" t="inlineStr"/>
@@ -3059,7 +3051,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>لقد تمت تعديل التقرير بنجاح</t>
+          <t>الاختصاص التعليمي</t>
         </is>
       </c>
       <c r="B329" t="inlineStr"/>
@@ -3067,7 +3059,7 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>لقد تم تعديل حالة البيان بنجاح</t>
+          <t>اسم الجهة الممولة</t>
         </is>
       </c>
       <c r="B330" t="inlineStr"/>
@@ -3075,7 +3067,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>لقد تم تعديل البيان بنجاح</t>
+          <t>عنوان الفرصة</t>
         </is>
       </c>
       <c r="B331" t="inlineStr"/>
@@ -3083,7 +3075,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>لقد تم حذف البيان بنجاح</t>
+          <t>وصف الفرصة</t>
         </is>
       </c>
       <c r="B332" t="inlineStr"/>
@@ -3091,7 +3083,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>لقد تمت إضافة المحتوى بنجاح و ستتم دراسته قريباً</t>
+          <t>نوع الفرصة</t>
         </is>
       </c>
       <c r="B333" t="inlineStr"/>
@@ -3099,7 +3091,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>لقد تم تعديل حالة المحتوى بنجاح</t>
+          <t>مكان الفرصة</t>
         </is>
       </c>
       <c r="B334" t="inlineStr"/>
@@ -3107,7 +3099,7 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>لقد تم تعديل المحتوى بنجاح</t>
+          <t>قطاع الفرصة</t>
         </is>
       </c>
       <c r="B335" t="inlineStr"/>
@@ -3115,7 +3107,7 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>لقد تم حذف المحتوى بنجاح</t>
+          <t>طريقة التقديم</t>
         </is>
       </c>
       <c r="B336" t="inlineStr"/>
@@ -3123,7 +3115,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>لقد تمت إضافة البحث بنجاح و ستتم دراسته قريباً</t>
+          <t>تطوير وإدارة المشاريع</t>
         </is>
       </c>
       <c r="B337" t="inlineStr"/>
@@ -3131,7 +3123,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>لقد تم تعديل حالة البحث بنجاح</t>
+          <t>الحوكمة التنظيمية</t>
         </is>
       </c>
       <c r="B338" t="inlineStr"/>
@@ -3139,7 +3131,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>لقد تم تعديل البحث بنجاح</t>
+          <t>المناصرة والحملات</t>
         </is>
       </c>
       <c r="B339" t="inlineStr"/>
@@ -3147,7 +3139,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>لقد تم حذف البحث بنجاح</t>
+          <t>مكتبة المجتمع المدني</t>
         </is>
       </c>
       <c r="B340" t="inlineStr"/>
@@ -3155,7 +3147,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>لقد تم تغيير حالة المنحة  بنجاح</t>
+          <t xml:space="preserve">اسم الجهة </t>
         </is>
       </c>
       <c r="B341" t="inlineStr"/>
@@ -3163,7 +3155,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>عربي</t>
+          <t>تاريخ الإعداد/النشر/التأليف</t>
         </is>
       </c>
       <c r="B342" t="inlineStr"/>
@@ -3171,7 +3163,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>English</t>
+          <t>لمحة عن الجهة</t>
         </is>
       </c>
       <c r="B343" t="inlineStr"/>
@@ -3179,7 +3171,7 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>Kurdî</t>
+          <t>موضوع المادة</t>
         </is>
       </c>
       <c r="B344" t="inlineStr"/>
@@ -3187,7 +3179,7 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>admin</t>
+          <t xml:space="preserve">المادة </t>
         </is>
       </c>
       <c r="B345" t="inlineStr"/>
@@ -3195,23 +3187,31 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>إضافة محافظة</t>
-        </is>
-      </c>
-      <c r="B346" t="inlineStr"/>
+          <t xml:space="preserve">تم إنشاء حسابك بنجاح باسم المستخدم ( {username} ) !, يرجى تأكيد عنوان بريدك الإلكتروني لإكمال التسجيل </t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Your Account has been created Successful with username ( {username} ) !, Please confirm your email address to complete the registration </t>
+        </is>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>احفظ</t>
-        </is>
-      </c>
-      <c r="B347" t="inlineStr"/>
+          <t>يرجى التسجيل باستخدام عنوان بريد إلكتروني آخر، هذا البريد الإلكتروني ( {user_email} ) مستخدم مسبقاً</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Please Sign-up with another email address, this email ( {user_email} ) is already in use</t>
+        </is>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>حذف محافظة</t>
+          <t>لقد تم حذف المحافظه بنجاح</t>
         </is>
       </c>
       <c r="B348" t="inlineStr"/>
@@ -3219,7 +3219,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t xml:space="preserve">هل أنت متأكد من رغبتك في حذف المحافظة </t>
+          <t>لقد تم تعديل الملف الشخصي بنجاح</t>
         </is>
       </c>
       <c r="B349" t="inlineStr"/>
@@ -3227,7 +3227,7 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>حذف المحافظة</t>
+          <t>لقد تم حذف الملف بنجاح</t>
         </is>
       </c>
       <c r="B350" t="inlineStr"/>
@@ -3235,7 +3235,7 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>عودة إلى الصفحة السابقة</t>
+          <t>لا يوجد حاليا منظمات</t>
         </is>
       </c>
       <c r="B351" t="inlineStr"/>
@@ -3243,7 +3243,7 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>تعديل محافظة</t>
+          <t>لا يوجد حالي أخبار</t>
         </is>
       </c>
       <c r="B352" t="inlineStr"/>
@@ -3251,7 +3251,7 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>محافظات دول الجوار لسوريا</t>
+          <t>لا يوجد حاليا فرص بناء</t>
         </is>
       </c>
       <c r="B353" t="inlineStr"/>
@@ -3259,7 +3259,7 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>المركز السوري للإعلام و حرية التعبير</t>
+          <t>لقد تم طلب الاشتراك بآخر اﻷخبار بنجاح</t>
         </is>
       </c>
       <c r="B354" t="inlineStr"/>
@@ -3267,7 +3267,7 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>بوابة المجتمع المدني</t>
+          <t>هذا البريد الالكتروني موجود مسبقاً يرجى التسجيل ببريد الكتروني أخر</t>
         </is>
       </c>
       <c r="B355" t="inlineStr"/>
@@ -3275,7 +3275,7 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>للتواصل معنا</t>
+          <t>لقد تم تغيير حالة الطلب للمنظمة بنجاح</t>
         </is>
       </c>
       <c r="B356" t="inlineStr"/>
@@ -3283,7 +3283,7 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>تابعونا على</t>
+          <t>لقد تمت إضافة الخبر بنجاح و ستتم دراسته قريباً</t>
         </is>
       </c>
       <c r="B357" t="inlineStr"/>
@@ -3291,7 +3291,7 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>للاشتراك بآخر الأخبار</t>
+          <t>لقد تم تغيير حالة الخبر بنجاح</t>
         </is>
       </c>
       <c r="B358" t="inlineStr"/>
@@ -3299,7 +3299,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>إملأ النموذج التالي</t>
+          <t>لقد تم تعديل الخبر بنجاح</t>
         </is>
       </c>
       <c r="B359" t="inlineStr"/>
@@ -3307,7 +3307,7 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>دليل المجتمع المدني</t>
+          <t>لقد تم حذف الخبر بنجاح</t>
         </is>
       </c>
       <c r="B360" t="inlineStr"/>
@@ -3315,7 +3315,7 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>أخبار المجتمع المدني</t>
+          <t>لقد تمت إضافة التقرير بنجاح و ستتم دراسته قريباً</t>
         </is>
       </c>
       <c r="B361" t="inlineStr"/>
@@ -3323,7 +3323,7 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>أخبار المنظمات</t>
+          <t>لقد تم تعديل حالة التقرير بنجاح</t>
         </is>
       </c>
       <c r="B362" t="inlineStr"/>
@@ -3331,7 +3331,7 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>تقارير ودراسات</t>
+          <t>لقد تم حذف التقرير بنجاح</t>
         </is>
       </c>
       <c r="B363" t="inlineStr"/>
@@ -3339,7 +3339,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>بيانات</t>
+          <t>لقد تمت تعديل التقرير بنجاح</t>
         </is>
       </c>
       <c r="B364" t="inlineStr"/>
@@ -3347,7 +3347,7 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>سمعي وبصري</t>
+          <t>لقد تمت إضافة البيان بنجاح و ستتم دراسته قريباً</t>
         </is>
       </c>
       <c r="B365" t="inlineStr"/>
@@ -3355,7 +3355,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>أبحاث خارجية</t>
+          <t>لقد تم تعديل حالة البيان بنجاح</t>
         </is>
       </c>
       <c r="B366" t="inlineStr"/>
@@ -3363,7 +3363,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>اﻷخبار</t>
+          <t>لقد تم تعديل البيان بنجاح</t>
         </is>
       </c>
       <c r="B367" t="inlineStr"/>
@@ -3371,7 +3371,7 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>موارد المجتمع المدني</t>
+          <t>لقد تم حذف البيان بنجاح</t>
         </is>
       </c>
       <c r="B368" t="inlineStr"/>
@@ -3379,7 +3379,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>فرص العمل</t>
+          <t>لقد تمت إضافة المحتوى بنجاح و ستتم دراسته قريباً</t>
         </is>
       </c>
       <c r="B369" t="inlineStr"/>
@@ -3387,7 +3387,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>فرص التمويل</t>
+          <t>لقد تم تعديل حالة المحتوى بنجاح</t>
         </is>
       </c>
       <c r="B370" t="inlineStr"/>
@@ -3395,7 +3395,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>فرص بناء القدرات</t>
+          <t>لقد تم تعديل المحتوى بنجاح</t>
         </is>
       </c>
       <c r="B371" t="inlineStr"/>
@@ -3403,7 +3403,7 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>دليل التطوير</t>
+          <t>لقد تم حذف المحتوى بنجاح</t>
         </is>
       </c>
       <c r="B372" t="inlineStr"/>
@@ -3411,7 +3411,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>الموارد</t>
+          <t>لقد تمت إضافة البحث بنجاح و ستتم دراسته قريباً</t>
         </is>
       </c>
       <c r="B373" t="inlineStr"/>
@@ -3419,7 +3419,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>أخبار البوابة</t>
+          <t>لقد تم تعديل حالة البحث بنجاح</t>
         </is>
       </c>
       <c r="B374" t="inlineStr"/>
@@ -3427,7 +3427,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>أهلاً</t>
+          <t>لقد تم تعديل البحث بنجاح</t>
         </is>
       </c>
       <c r="B375" t="inlineStr"/>
@@ -3435,7 +3435,7 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>لوحة التحكم الخاصة باﻹدارة</t>
+          <t>لقد تم حذف البحث بنجاح</t>
         </is>
       </c>
       <c r="B376" t="inlineStr"/>
@@ -3443,7 +3443,7 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>ملفي الشخصي</t>
+          <t>لقد تمت إضافة فرصة العمل بنجاح و ستتم دراستها قريباً</t>
         </is>
       </c>
       <c r="B377" t="inlineStr"/>
@@ -3451,7 +3451,7 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>تغيير كلمة المرور</t>
+          <t>يجب إدخال اسم منظمة لتتم معالجة و نشر فرصة العمل</t>
         </is>
       </c>
       <c r="B378" t="inlineStr"/>
@@ -3459,7 +3459,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>تسجيل الخروج</t>
+          <t>لقد تم تغيير حالة فرصة العمل بنجاح</t>
         </is>
       </c>
       <c r="B379" t="inlineStr"/>
@@ -3467,7 +3467,7 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>تسجيل الدخول</t>
+          <t>لقد تم تعديل فرصة العمل بنجاح</t>
         </is>
       </c>
       <c r="B380" t="inlineStr"/>
@@ -3475,7 +3475,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>تقديم طلب اشتراك جديد لمنظمة</t>
+          <t>لقد تم حذف فرصة العمل بنجاح</t>
         </is>
       </c>
       <c r="B381" t="inlineStr"/>
@@ -3483,7 +3483,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>طلبات المنظمات قيد الدراسة</t>
+          <t>لقد تم تسجيل طلب فرصة التمويل بنجاح و ستتم دراسته قريباً</t>
         </is>
       </c>
       <c r="B382" t="inlineStr"/>
@@ -3491,7 +3491,7 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>طلبات المنظمات الموافق عليها</t>
+          <t>رجاءً أدخل اسم المنظمة أو الجهة المانحة لتتم دراسة فرصة التمويل</t>
         </is>
       </c>
       <c r="B383" t="inlineStr"/>
@@ -3499,7 +3499,7 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>إضافة خبر لمنظمة</t>
+          <t>لقد تم تغيير حالة فرصة التمويل بنجاح</t>
         </is>
       </c>
       <c r="B384" t="inlineStr"/>
@@ -3507,7 +3507,7 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>أخبار المنظمات قيد الدراسة</t>
+          <t>لقد تم تعديل فرصة التمويل بنجاح</t>
         </is>
       </c>
       <c r="B385" t="inlineStr"/>
@@ -3515,7 +3515,7 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>إضافة تقرير أو دراسة لمنظمة</t>
+          <t>لقد تم حذف فرصة التمويل بنجاح</t>
         </is>
       </c>
       <c r="B386" t="inlineStr"/>
@@ -3523,7 +3523,7 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>تقارير و دراسات المنظمات قيد الدراسة</t>
+          <t>لقد تمت إضافة فرصة التمويل بنجاح و ستتم دراسته قريباً</t>
         </is>
       </c>
       <c r="B387" t="inlineStr"/>
@@ -3531,7 +3531,7 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>إضافة بيان لمنظمة</t>
+          <t>يحب إدخال اسم منظمة أو اسم الجهة المانحة لنتمكن من دراسة فرصة التمويل</t>
         </is>
       </c>
       <c r="B388" t="inlineStr"/>
@@ -3539,7 +3539,7 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>بيانات المنظمات قيد الدراسة</t>
+          <t>لقد تم تغيير حالة المنحة  بنجاح</t>
         </is>
       </c>
       <c r="B389" t="inlineStr"/>
@@ -3547,7 +3547,7 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>إضافة محتوى سمعي و بصري لمنظمة</t>
+          <t>لقد تمت إضافة فرصة بناء القدرات بنجاح و ستتم دراسته قريباً</t>
         </is>
       </c>
       <c r="B390" t="inlineStr"/>
@@ -3555,7 +3555,7 @@
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>المحتوى السمعي و البصري للمنظمات قيد الدراسة</t>
+          <t>يجب إدخال اسم الجهة المانحة لنتمكن من دراسة الفرصة</t>
         </is>
       </c>
       <c r="B391" t="inlineStr"/>
@@ -3563,7 +3563,7 @@
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>إضافة بحث خارجي لمنظمة</t>
+          <t>لقد تم تغيير حالة فرصة بناء القدرات  بنجاح</t>
         </is>
       </c>
       <c r="B392" t="inlineStr"/>
@@ -3571,7 +3571,7 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>اﻷبحاث الخارجية للمنظمات قيد الدراسة</t>
+          <t>لقد تم تعديل فرصة بناء القدرات بنجاح</t>
         </is>
       </c>
       <c r="B393" t="inlineStr"/>
@@ -3579,7 +3579,7 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>إضافة فرصة عمل</t>
+          <t>لقد تم حذف فرصة بناء القدرات بنجاح</t>
         </is>
       </c>
       <c r="B394" t="inlineStr"/>
@@ -3587,7 +3587,7 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>فرص العمل للمنظمات قيد الدراسة</t>
+          <t>لقد تمت إضافة دليل تطوير بنجاح و ستتم دراسته قريباً</t>
         </is>
       </c>
       <c r="B395" t="inlineStr"/>
@@ -3595,7 +3595,7 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>إضافة فرصة تمويل</t>
+          <t>لقد تم تغيير حالة دليل تطوير بنجاح</t>
         </is>
       </c>
       <c r="B396" t="inlineStr"/>
@@ -3603,7 +3603,7 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>فرص التمويل للمنظمات قيد الدراسة</t>
+          <t>لقد تم تعديل دليل التطوير بنجاح</t>
         </is>
       </c>
       <c r="B397" t="inlineStr"/>
@@ -3611,7 +3611,7 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>إضافة فرصة بناء القدرات</t>
+          <t>عربي</t>
         </is>
       </c>
       <c r="B398" t="inlineStr"/>
@@ -3619,7 +3619,7 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>فرص بناء القدرات للمنظمات قيد الدراسة</t>
+          <t>English</t>
         </is>
       </c>
       <c r="B399" t="inlineStr"/>
@@ -3627,7 +3627,7 @@
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>إضافة دليل تطوير</t>
+          <t>Kurdî</t>
         </is>
       </c>
       <c r="B400" t="inlineStr"/>
@@ -3635,7 +3635,7 @@
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>دليل التطوير للمنظمات قيد الدراسة</t>
+          <t>admin</t>
         </is>
       </c>
       <c r="B401" t="inlineStr"/>
@@ -3643,7 +3643,7 @@
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>اتصل بنا</t>
+          <t>إضافة محافظة</t>
         </is>
       </c>
       <c r="B402" t="inlineStr"/>
@@ -3651,7 +3651,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>خطأ 404 , صفحة غير متاحة</t>
+          <t>احفظ</t>
         </is>
       </c>
       <c r="B403" t="inlineStr"/>
@@ -3659,7 +3659,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>صفحة غير متاحة</t>
+          <t>حذف محافظة</t>
         </is>
       </c>
       <c r="B404" t="inlineStr"/>
@@ -3667,7 +3667,7 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>هذه الصفحة مفقودة أو غير متوفره أساساً</t>
+          <t xml:space="preserve">هل أنت متأكد من رغبتك في حذف المحافظة </t>
         </is>
       </c>
       <c r="B405" t="inlineStr"/>
@@ -3675,7 +3675,7 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>العودة إلى الصفحة الرئيسية</t>
+          <t>حذف المحافظة</t>
         </is>
       </c>
       <c r="B406" t="inlineStr"/>
@@ -3683,7 +3683,7 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>فرص بناء القدرات  قيد الدراسة</t>
+          <t>عودة إلى الصفحة السابقة</t>
         </is>
       </c>
       <c r="B407" t="inlineStr"/>
@@ -3691,7 +3691,7 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>لقراءة المزيد</t>
+          <t>تعديل محافظة</t>
         </is>
       </c>
       <c r="B408" t="inlineStr"/>
@@ -3699,7 +3699,7 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>لا يوجد حالياً فرص بناء قدرات للنشر</t>
+          <t>محافظات دول الجوار لسوريا</t>
         </is>
       </c>
       <c r="B409" t="inlineStr"/>
@@ -3707,7 +3707,7 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>اضافة فرصة بناء القدرات</t>
+          <t>المركز السوري للإعلام و حرية التعبير</t>
         </is>
       </c>
       <c r="B410" t="inlineStr"/>
@@ -3715,7 +3715,7 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>انشر فرصة بناء قدرات</t>
+          <t>بوابة المجتمع المدني</t>
         </is>
       </c>
       <c r="B411" t="inlineStr"/>
@@ -3723,7 +3723,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>فرز</t>
+          <t>للتواصل معنا</t>
         </is>
       </c>
       <c r="B412" t="inlineStr"/>
@@ -3731,7 +3731,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>فرص بناء القدرات قيد الدراسة</t>
+          <t>تابعونا على</t>
         </is>
       </c>
       <c r="B413" t="inlineStr"/>
@@ -3739,7 +3739,7 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>بحث</t>
+          <t>للاشتراك بآخر الأخبار</t>
         </is>
       </c>
       <c r="B414" t="inlineStr"/>
@@ -3747,7 +3747,7 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t xml:space="preserve"> لا يوجد حالياً فرص بناء القدرات </t>
+          <t>إملأ النموذج التالي</t>
         </is>
       </c>
       <c r="B415" t="inlineStr"/>
@@ -3755,7 +3755,7 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>حذف فرصة بناء القدرات</t>
+          <t>دليل المجتمع المدني</t>
         </is>
       </c>
       <c r="B416" t="inlineStr"/>
@@ -3763,7 +3763,7 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>هل أنت متأكد من رغبتك في حذف فرصة بناء القدرات بعنوان</t>
+          <t>أخبار المجتمع المدني</t>
         </is>
       </c>
       <c r="B417" t="inlineStr"/>
@@ -3771,7 +3771,7 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>حذف</t>
+          <t>أخبار المنظمات</t>
         </is>
       </c>
       <c r="B418" t="inlineStr"/>
@@ -3779,7 +3779,7 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>تفاصيل فرصة بناء القدرات</t>
+          <t>تقارير ودراسات</t>
         </is>
       </c>
       <c r="B419" t="inlineStr"/>
@@ -3787,7 +3787,7 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>اسم اللذي أضاف فرصة بناء القدرات</t>
+          <t>بيانات</t>
         </is>
       </c>
       <c r="B420" t="inlineStr"/>
@@ -3795,7 +3795,7 @@
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t xml:space="preserve">  تاريخ الإضافة </t>
+          <t>سمعي وبصري</t>
         </is>
       </c>
       <c r="B421" t="inlineStr"/>
@@ -3803,7 +3803,7 @@
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>وصف فرصة التمويل</t>
+          <t>أبحاث خارجية</t>
         </is>
       </c>
       <c r="B422" t="inlineStr"/>
@@ -3811,7 +3811,7 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t xml:space="preserve">الموافقة على نشر </t>
+          <t>اﻷخبار</t>
         </is>
       </c>
       <c r="B423" t="inlineStr"/>
@@ -3819,7 +3819,7 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>إلغاء نشر الخبر</t>
+          <t>موارد المجتمع المدني</t>
         </is>
       </c>
       <c r="B424" t="inlineStr"/>
@@ -3827,7 +3827,7 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>تعديل فرصة بناءالقدرات</t>
+          <t>فرص العمل</t>
         </is>
       </c>
       <c r="B425" t="inlineStr"/>
@@ -3835,7 +3835,7 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t xml:space="preserve">حذف </t>
+          <t>فرص التمويل</t>
         </is>
       </c>
       <c r="B426" t="inlineStr"/>
@@ -3843,7 +3843,7 @@
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t xml:space="preserve"> تعديل فرصة بناء القدرات</t>
+          <t>فرص بناء القدرات</t>
         </is>
       </c>
       <c r="B427" t="inlineStr"/>
@@ -3851,7 +3851,7 @@
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>تعديل فرصة بناء القدرات</t>
+          <t>دليل التطوير</t>
         </is>
       </c>
       <c r="B428" t="inlineStr"/>
@@ -3859,7 +3859,7 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>تعديل</t>
+          <t>الموارد</t>
         </is>
       </c>
       <c r="B429" t="inlineStr"/>
@@ -3867,7 +3867,7 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>أخبار المركز</t>
+          <t>أخبار البوابة</t>
         </is>
       </c>
       <c r="B430" t="inlineStr"/>
@@ -3875,7 +3875,7 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>إضافة خبر</t>
+          <t>أهلاً</t>
         </is>
       </c>
       <c r="B431" t="inlineStr"/>
@@ -3883,7 +3883,7 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>نص الخبر</t>
+          <t>لوحة التحكم الخاصة باﻹدارة</t>
         </is>
       </c>
       <c r="B432" t="inlineStr"/>
@@ -3891,7 +3891,7 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>أضف صورة الخبر</t>
+          <t>ملفي الشخصي</t>
         </is>
       </c>
       <c r="B433" t="inlineStr"/>
@@ -3899,7 +3899,7 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>أضف</t>
+          <t>تغيير كلمة المرور</t>
         </is>
       </c>
       <c r="B434" t="inlineStr"/>
@@ -3907,7 +3907,7 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>تاريخ الخبر</t>
+          <t>تسجيل الخروج</t>
         </is>
       </c>
       <c r="B435" t="inlineStr"/>
@@ -3915,7 +3915,7 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>مشاركة على فيسبوك</t>
+          <t>تسجيل الدخول</t>
         </is>
       </c>
       <c r="B436" t="inlineStr"/>
@@ -3923,7 +3923,7 @@
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>عودة إلى صفحة أخبار المركز</t>
+          <t>تقديم طلب اشتراك جديد لمنظمة</t>
         </is>
       </c>
       <c r="B437" t="inlineStr"/>
@@ -3931,7 +3931,7 @@
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>إضافة بيان</t>
+          <t>طلبات المنظمات قيد الدراسة</t>
         </is>
       </c>
       <c r="B438" t="inlineStr"/>
@@ -3939,7 +3939,7 @@
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>البيانات</t>
+          <t>طلبات المنظمات الموافق عليها</t>
         </is>
       </c>
       <c r="B439" t="inlineStr"/>
@@ -3947,7 +3947,7 @@
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t xml:space="preserve"> لا يوجد حالياً بيانات منشورة للمنظمات</t>
+          <t>إضافة خبر لمنظمة</t>
         </is>
       </c>
       <c r="B440" t="inlineStr"/>
@@ -3955,7 +3955,7 @@
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>بيانات قيد الدراسة</t>
+          <t>أخبار المنظمات قيد الدراسة</t>
         </is>
       </c>
       <c r="B441" t="inlineStr"/>
@@ -3963,7 +3963,7 @@
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t xml:space="preserve"> لا يوجد حالياً بيانات قيد الدراسة منشورة للمنظمات</t>
+          <t>إضافة تقرير أو دراسة لمنظمة</t>
         </is>
       </c>
       <c r="B442" t="inlineStr"/>
@@ -3971,7 +3971,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>حذف البيان</t>
+          <t>تقارير و دراسات المنظمات قيد الدراسة</t>
         </is>
       </c>
       <c r="B443" t="inlineStr"/>
@@ -3979,7 +3979,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>هل أنت متأكد من رغبتك في حذف البيان بعنوان</t>
+          <t>إضافة بيان لمنظمة</t>
         </is>
       </c>
       <c r="B444" t="inlineStr"/>
@@ -3987,7 +3987,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>تفاصيل البيان</t>
+          <t>بيانات المنظمات قيد الدراسة</t>
         </is>
       </c>
       <c r="B445" t="inlineStr"/>
@@ -3995,7 +3995,7 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>اسم اللذي أضاف البيان</t>
+          <t>إضافة محتوى سمعي و بصري لمنظمة</t>
         </is>
       </c>
       <c r="B446" t="inlineStr"/>
@@ -4003,7 +4003,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>تاريخ إضافة البيان</t>
+          <t>المحتوى السمعي و البصري للمنظمات قيد الدراسة</t>
         </is>
       </c>
       <c r="B447" t="inlineStr"/>
@@ -4011,7 +4011,7 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>محتوى البيان</t>
+          <t>إضافة بحث خارجي لمنظمة</t>
         </is>
       </c>
       <c r="B448" t="inlineStr"/>
@@ -4019,7 +4019,7 @@
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>الموافقة على نشر البيان</t>
+          <t>اﻷبحاث الخارجية للمنظمات قيد الدراسة</t>
         </is>
       </c>
       <c r="B449" t="inlineStr"/>
@@ -4027,7 +4027,7 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>إلغاء نشر البيان</t>
+          <t>إضافة فرصة عمل</t>
         </is>
       </c>
       <c r="B450" t="inlineStr"/>
@@ -4035,7 +4035,7 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>تعديل البيان</t>
+          <t>فرص العمل للمنظمات قيد الدراسة</t>
         </is>
       </c>
       <c r="B451" t="inlineStr"/>
@@ -4043,7 +4043,7 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>لا يوجد حالياً دليل تطوير</t>
+          <t>إضافة فرصة تمويل</t>
         </is>
       </c>
       <c r="B452" t="inlineStr"/>
@@ -4051,7 +4051,7 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>إضافة</t>
+          <t>فرص التمويل للمنظمات قيد الدراسة</t>
         </is>
       </c>
       <c r="B453" t="inlineStr"/>
@@ -4059,7 +4059,7 @@
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>اضافة دليل تطوير</t>
+          <t>إضافة فرصة بناء القدرات</t>
         </is>
       </c>
       <c r="B454" t="inlineStr"/>
@@ -4067,7 +4067,7 @@
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>انشر دليل التطوير</t>
+          <t>فرص بناء القدرات للمنظمات قيد الدراسة</t>
         </is>
       </c>
       <c r="B455" t="inlineStr"/>
@@ -4075,7 +4075,7 @@
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>حذف الدليل</t>
+          <t>إضافة دليل تطوير</t>
         </is>
       </c>
       <c r="B456" t="inlineStr"/>
@@ -4083,7 +4083,7 @@
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>حذف دليل التطوير</t>
+          <t>دليل التطوير للمنظمات قيد الدراسة</t>
         </is>
       </c>
       <c r="B457" t="inlineStr"/>
@@ -4091,7 +4091,7 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>هل أنت متأكد من رغبتك في حذف دليل التطوير بعنوان</t>
+          <t>اتصل بنا</t>
         </is>
       </c>
       <c r="B458" t="inlineStr"/>
@@ -4099,7 +4099,7 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>تفاصيل دليل التطوير</t>
+          <t>خطأ 404 , صفحة غير متاحة</t>
         </is>
       </c>
       <c r="B459" t="inlineStr"/>
@@ -4107,7 +4107,7 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>اسم اللذي أضاف  تفاصيل دليل التطوير</t>
+          <t>صفحة غير متاحة</t>
         </is>
       </c>
       <c r="B460" t="inlineStr"/>
@@ -4115,7 +4115,7 @@
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>عنوان</t>
+          <t>هذه الصفحة مفقودة أو غير متوفره أساساً</t>
         </is>
       </c>
       <c r="B461" t="inlineStr"/>
@@ -4123,7 +4123,7 @@
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>وصف الدليل</t>
+          <t>العودة إلى الصفحة الرئيسية</t>
         </is>
       </c>
       <c r="B462" t="inlineStr"/>
@@ -4131,7 +4131,7 @@
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t xml:space="preserve">الموافقة على النشر </t>
+          <t>فرص بناء القدرات  قيد الدراسة</t>
         </is>
       </c>
       <c r="B463" t="inlineStr"/>
@@ -4139,7 +4139,7 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>إلغاء نشر الدليل</t>
+          <t>لقراءة المزيد</t>
         </is>
       </c>
       <c r="B464" t="inlineStr"/>
@@ -4147,7 +4147,7 @@
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>تعديل الدليل</t>
+          <t>لا يوجد حالياً فرص بناء قدرات للنشر</t>
         </is>
       </c>
       <c r="B465" t="inlineStr"/>
@@ -4155,7 +4155,7 @@
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>اضافة دليل التطوير</t>
+          <t>اضافة فرصة بناء القدرات</t>
         </is>
       </c>
       <c r="B466" t="inlineStr"/>
@@ -4163,7 +4163,7 @@
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>دليل التطوير قيد الدراسة</t>
+          <t>انشر فرصة بناء قدرات</t>
         </is>
       </c>
       <c r="B467" t="inlineStr"/>
@@ -4171,7 +4171,7 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>لا يوجد حالياً دليل تطوير منشور من قبل المنظمات</t>
+          <t>فرز</t>
         </is>
       </c>
       <c r="B468" t="inlineStr"/>
@@ -4179,7 +4179,7 @@
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>تعديل دليل التطوير</t>
+          <t>فرص بناء القدرات قيد الدراسة</t>
         </is>
       </c>
       <c r="B469" t="inlineStr"/>
@@ -4187,7 +4187,7 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>فرص التمويل قيد الدراسة</t>
+          <t>بحث</t>
         </is>
       </c>
       <c r="B470" t="inlineStr"/>
@@ -4195,7 +4195,7 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>لا يوجد حالياً فرص فرص تمويل للموافقة على النشر</t>
+          <t xml:space="preserve"> لا يوجد حالياً فرص بناء القدرات </t>
         </is>
       </c>
       <c r="B471" t="inlineStr"/>
@@ -4203,7 +4203,7 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>اضافة فرصة تمويل</t>
+          <t>حذف فرصة بناء القدرات</t>
         </is>
       </c>
       <c r="B472" t="inlineStr"/>
@@ -4211,7 +4211,7 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>اضافة</t>
+          <t>هل أنت متأكد من رغبتك في حذف فرصة بناء القدرات بعنوان</t>
         </is>
       </c>
       <c r="B473" t="inlineStr"/>
@@ -4219,7 +4219,7 @@
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>تعديل فرصة التمويل</t>
+          <t>حذف</t>
         </is>
       </c>
       <c r="B474" t="inlineStr"/>
@@ -4227,7 +4227,7 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>لا يوجد حالياً فرص تمويل منشورة من قبل المنظمات</t>
+          <t>تفاصيل فرصة بناء القدرات</t>
         </is>
       </c>
       <c r="B475" t="inlineStr"/>
@@ -4235,7 +4235,7 @@
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>حذف فرصةالتمويل</t>
+          <t>اسم اللذي أضاف فرصة بناء القدرات</t>
         </is>
       </c>
       <c r="B476" t="inlineStr"/>
@@ -4243,7 +4243,7 @@
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>هل أنت متأكد من رغبتك في حذف فرصةالتمويل بعنوان</t>
+          <t>اسم الجهة المانحة</t>
         </is>
       </c>
       <c r="B477" t="inlineStr"/>
@@ -4251,7 +4251,7 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>تفاصيل فرصة التمويل</t>
+          <t>تاريخ الإضافة</t>
         </is>
       </c>
       <c r="B478" t="inlineStr"/>
@@ -4259,7 +4259,7 @@
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>اسم اللذي أضاف فرصة التمويل</t>
+          <t>وصف فرصة التمويل</t>
         </is>
       </c>
       <c r="B479" t="inlineStr"/>
@@ -4267,7 +4267,7 @@
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>الموافقة على النشر</t>
+          <t>لم يذكر</t>
         </is>
       </c>
       <c r="B480" t="inlineStr"/>
@@ -4275,7 +4275,7 @@
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>إلغاء نشر فرصة التمويل</t>
+          <t xml:space="preserve">الموافقة على نشر </t>
         </is>
       </c>
       <c r="B481" t="inlineStr"/>
@@ -4283,7 +4283,7 @@
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>قائمة دليل المجتمع المدني للموافقة على النشر</t>
+          <t>إلغاء نشر الخبر</t>
         </is>
       </c>
       <c r="B482" t="inlineStr"/>
@@ -4291,7 +4291,7 @@
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>للمزيد عن المنظمة</t>
+          <t>تعديل فرصة بناءالقدرات</t>
         </is>
       </c>
       <c r="B483" t="inlineStr"/>
@@ -4299,7 +4299,7 @@
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>حالياً لا يوجد طلبات للمنظمات للموافقة عليها</t>
+          <t xml:space="preserve">حذف </t>
         </is>
       </c>
       <c r="B484" t="inlineStr"/>
@@ -4307,7 +4307,7 @@
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>عودة إلى صفحة دليل المنظمات</t>
+          <t xml:space="preserve"> تعديل فرصة بناء القدرات</t>
         </is>
       </c>
       <c r="B485" t="inlineStr"/>
@@ -4315,7 +4315,7 @@
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>إقراء المزيد</t>
+          <t>تعديل فرصة بناء القدرات</t>
         </is>
       </c>
       <c r="B486" t="inlineStr"/>
@@ -4323,7 +4323,7 @@
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>قائمة منظمات المجتمع المدني</t>
+          <t>تعديل</t>
         </is>
       </c>
       <c r="B487" t="inlineStr"/>
@@ -4331,7 +4331,7 @@
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>طلبات اشتراك المنظمات قيد الدراسة</t>
+          <t>أخبار المركز</t>
         </is>
       </c>
       <c r="B488" t="inlineStr"/>
@@ -4339,7 +4339,7 @@
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>إجمالي عدد المنظمات</t>
+          <t>إضافة خبر</t>
         </is>
       </c>
       <c r="B489" t="inlineStr"/>
@@ -4347,7 +4347,7 @@
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>حالياً لا يوجد منظمات مسجله او موافق عليها</t>
+          <t>نص الخبر</t>
         </is>
       </c>
       <c r="B490" t="inlineStr"/>
@@ -4355,7 +4355,7 @@
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t>دليل المجتمع المدني بحسب مجال العمل</t>
+          <t>أضف صورة الخبر</t>
         </is>
       </c>
       <c r="B491" t="inlineStr"/>
@@ -4363,7 +4363,7 @@
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t>المنظمات المضافة حديثاً</t>
+          <t>أضف</t>
         </is>
       </c>
       <c r="B492" t="inlineStr"/>
@@ -4371,7 +4371,7 @@
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>أحدث اﻷخبار</t>
+          <t>تاريخ الخبر</t>
         </is>
       </c>
       <c r="B493" t="inlineStr"/>
@@ -4379,7 +4379,7 @@
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>للمزيد عن الخبر</t>
+          <t>مشاركة على فيسبوك</t>
         </is>
       </c>
       <c r="B494" t="inlineStr"/>
@@ -4387,7 +4387,7 @@
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>أحدث فرص العمل</t>
+          <t>عودة إلى صفحة أخبار المركز</t>
         </is>
       </c>
       <c r="B495" t="inlineStr"/>
@@ -4395,7 +4395,7 @@
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>للمزيد عن فرصة العمل</t>
+          <t>إضافة بيان</t>
         </is>
       </c>
       <c r="B496" t="inlineStr"/>
@@ -4403,7 +4403,7 @@
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t>أحدث فرص بناء القدرات</t>
+          <t>البيانات</t>
         </is>
       </c>
       <c r="B497" t="inlineStr"/>
@@ -4411,7 +4411,7 @@
     <row r="498">
       <c r="A498" t="inlineStr">
         <is>
-          <t>للمزيد عن فرصة بناء القدرات</t>
+          <t xml:space="preserve"> لا يوجد حالياً بيانات منشورة للمنظمات</t>
         </is>
       </c>
       <c r="B498" t="inlineStr"/>
@@ -4419,7 +4419,7 @@
     <row r="499">
       <c r="A499" t="inlineStr">
         <is>
-          <t>اشترك</t>
+          <t>بيانات قيد الدراسة</t>
         </is>
       </c>
       <c r="B499" t="inlineStr"/>
@@ -4427,7 +4427,7 @@
     <row r="500">
       <c r="A500" t="inlineStr">
         <is>
-          <t>إضافة محتوى سمعي و بصري</t>
+          <t xml:space="preserve"> لا يوجد حالياً بيانات قيد الدراسة منشورة للمنظمات</t>
         </is>
       </c>
       <c r="B500" t="inlineStr"/>
@@ -4435,7 +4435,7 @@
     <row r="501">
       <c r="A501" t="inlineStr">
         <is>
-          <t>حذف المحتوى السمعي و البصري</t>
+          <t>حذف البيان</t>
         </is>
       </c>
       <c r="B501" t="inlineStr"/>
@@ -4443,7 +4443,7 @@
     <row r="502">
       <c r="A502" t="inlineStr">
         <is>
-          <t>هل أنت متأكد من رغبتك في حذف المحتوى بعنوان</t>
+          <t>هل أنت متأكد من رغبتك في حذف البيان بعنوان</t>
         </is>
       </c>
       <c r="B502" t="inlineStr"/>
@@ -4451,7 +4451,7 @@
     <row r="503">
       <c r="A503" t="inlineStr">
         <is>
-          <t>حذف المحتوى</t>
+          <t>تفاصيل البيان</t>
         </is>
       </c>
       <c r="B503" t="inlineStr"/>
@@ -4459,7 +4459,7 @@
     <row r="504">
       <c r="A504" t="inlineStr">
         <is>
-          <t>تعديل المحتوى السمعي و البصري</t>
+          <t>اسم اللذي أضاف البيان</t>
         </is>
       </c>
       <c r="B504" t="inlineStr"/>
@@ -4467,7 +4467,7 @@
     <row r="505">
       <c r="A505" t="inlineStr">
         <is>
-          <t>المحتوى السمعي و البصري</t>
+          <t>تاريخ إضافة البيان</t>
         </is>
       </c>
       <c r="B505" t="inlineStr"/>
@@ -4475,7 +4475,7 @@
     <row r="506">
       <c r="A506" t="inlineStr">
         <is>
-          <t xml:space="preserve"> لا يوجد حالياً محتوى سمعي و بصري منشور من قبل المنظمات</t>
+          <t>محتوى البيان</t>
         </is>
       </c>
       <c r="B506" t="inlineStr"/>
@@ -4483,7 +4483,7 @@
     <row r="507">
       <c r="A507" t="inlineStr">
         <is>
-          <t>تفاصيل المحتوى السمعي والبصري</t>
+          <t>الموافقة على نشر البيان</t>
         </is>
       </c>
       <c r="B507" t="inlineStr"/>
@@ -4491,7 +4491,7 @@
     <row r="508">
       <c r="A508" t="inlineStr">
         <is>
-          <t>اسم اللذي أضاف المحتوى</t>
+          <t>إلغاء نشر البيان</t>
         </is>
       </c>
       <c r="B508" t="inlineStr"/>
@@ -4499,7 +4499,7 @@
     <row r="509">
       <c r="A509" t="inlineStr">
         <is>
-          <t>تاريخ إضافة المحتوى</t>
+          <t>تعديل البيان</t>
         </is>
       </c>
       <c r="B509" t="inlineStr"/>
@@ -4507,7 +4507,7 @@
     <row r="510">
       <c r="A510" t="inlineStr">
         <is>
-          <t>مضمون المحتوى السمعي و البصري</t>
+          <t>لا يوجد حالياً دليل تطوير</t>
         </is>
       </c>
       <c r="B510" t="inlineStr"/>
@@ -4515,7 +4515,7 @@
     <row r="511">
       <c r="A511" t="inlineStr">
         <is>
-          <t>الموافقة على نشر المحتوى</t>
+          <t>اضافة دليل تطوير</t>
         </is>
       </c>
       <c r="B511" t="inlineStr"/>
@@ -4523,7 +4523,7 @@
     <row r="512">
       <c r="A512" t="inlineStr">
         <is>
-          <t>إلغاء نشر المحتوى</t>
+          <t>انشر دليل التطوير</t>
         </is>
       </c>
       <c r="B512" t="inlineStr"/>
@@ -4531,7 +4531,7 @@
     <row r="513">
       <c r="A513" t="inlineStr">
         <is>
-          <t>تعديل المحتوى</t>
+          <t>حذف الدليل</t>
         </is>
       </c>
       <c r="B513" t="inlineStr"/>
@@ -4539,7 +4539,7 @@
     <row r="514">
       <c r="A514" t="inlineStr">
         <is>
-          <t>المحتوى السمعي و البصري قيد الدراسة</t>
+          <t>حذف دليل التطوير</t>
         </is>
       </c>
       <c r="B514" t="inlineStr"/>
@@ -4547,7 +4547,7 @@
     <row r="515">
       <c r="A515" t="inlineStr">
         <is>
-          <t>لا يوجد حالياً محتوى سمعي و بصري منشور من قبل المنظمات للموافقة على النشر</t>
+          <t>هل أنت متأكد من رغبتك في حذف دليل التطوير بعنوان</t>
         </is>
       </c>
       <c r="B515" t="inlineStr"/>
@@ -4555,7 +4555,7 @@
     <row r="516">
       <c r="A516" t="inlineStr">
         <is>
-          <t>انشر الخبر</t>
+          <t>تفاصيل دليل التطوير</t>
         </is>
       </c>
       <c r="B516" t="inlineStr"/>
@@ -4563,7 +4563,7 @@
     <row r="517">
       <c r="A517" t="inlineStr">
         <is>
-          <t>تعديل خبر</t>
+          <t>اسم اللذي أضاف  تفاصيل دليل التطوير</t>
         </is>
       </c>
       <c r="B517" t="inlineStr"/>
@@ -4571,7 +4571,7 @@
     <row r="518">
       <c r="A518" t="inlineStr">
         <is>
-          <t>تعديل الخبر</t>
+          <t xml:space="preserve">  تاريخ الإضافة </t>
         </is>
       </c>
       <c r="B518" t="inlineStr"/>
@@ -4579,7 +4579,7 @@
     <row r="519">
       <c r="A519" t="inlineStr">
         <is>
-          <t>حذف خبر</t>
+          <t>عنوان</t>
         </is>
       </c>
       <c r="B519" t="inlineStr"/>
@@ -4587,7 +4587,7 @@
     <row r="520">
       <c r="A520" t="inlineStr">
         <is>
-          <t xml:space="preserve">هل أنت متأكد من رغبتك في حذف الخبر بعنوان </t>
+          <t>وصف الدليل</t>
         </is>
       </c>
       <c r="B520" t="inlineStr"/>
@@ -4595,7 +4595,7 @@
     <row r="521">
       <c r="A521" t="inlineStr">
         <is>
-          <t>حذف الخبر</t>
+          <t>المادة</t>
         </is>
       </c>
       <c r="B521" t="inlineStr"/>
@@ -4603,7 +4603,7 @@
     <row r="522">
       <c r="A522" t="inlineStr">
         <is>
-          <t>لا يوجد حالياً أخبار للموافقة على النشر</t>
+          <t xml:space="preserve">الموافقة على النشر </t>
         </is>
       </c>
       <c r="B522" t="inlineStr"/>
@@ -4611,7 +4611,7 @@
     <row r="523">
       <c r="A523" t="inlineStr">
         <is>
-          <t>تاريخ إضافة الخبر</t>
+          <t>إلغاء نشر الدليل</t>
         </is>
       </c>
       <c r="B523" t="inlineStr"/>
@@ -4619,7 +4619,7 @@
     <row r="524">
       <c r="A524" t="inlineStr">
         <is>
-          <t>اسم اللذي أضاف الخبر</t>
+          <t>تعديل الدليل</t>
         </is>
       </c>
       <c r="B524" t="inlineStr"/>
@@ -4627,7 +4627,7 @@
     <row r="525">
       <c r="A525" t="inlineStr">
         <is>
-          <t>أحدث ثلاثة أخبار</t>
+          <t>اضافة دليل التطوير</t>
         </is>
       </c>
       <c r="B525" t="inlineStr"/>
@@ -4635,7 +4635,7 @@
     <row r="526">
       <c r="A526" t="inlineStr">
         <is>
-          <t>الموافقة على نشر الخبر</t>
+          <t>دليل التطوير قيد الدراسة</t>
         </is>
       </c>
       <c r="B526" t="inlineStr"/>
@@ -4643,7 +4643,7 @@
     <row r="527">
       <c r="A527" t="inlineStr">
         <is>
-          <t>لا يوجد حالياً أخبار منشورة للمنظمات</t>
+          <t>لا يوجد حالياً دليل تطوير منشور من قبل المنظمات</t>
         </is>
       </c>
       <c r="B527" t="inlineStr"/>
@@ -4651,7 +4651,7 @@
     <row r="528">
       <c r="A528" t="inlineStr">
         <is>
-          <t>اخبار البوابة</t>
+          <t>تعديل دليل التطوير</t>
         </is>
       </c>
       <c r="B528" t="inlineStr"/>
@@ -4659,7 +4659,7 @@
     <row r="529">
       <c r="A529" t="inlineStr">
         <is>
-          <t xml:space="preserve">اخبار البوابة </t>
+          <t>فرص تمويل المنظمات</t>
         </is>
       </c>
       <c r="B529" t="inlineStr"/>
@@ -4667,7 +4667,7 @@
     <row r="530">
       <c r="A530" t="inlineStr">
         <is>
-          <t>أخبار البوابةقيد الدراسة</t>
+          <t>فرص تمويل الأفراد</t>
         </is>
       </c>
       <c r="B530" t="inlineStr"/>
@@ -4675,7 +4675,7 @@
     <row r="531">
       <c r="A531" t="inlineStr">
         <is>
-          <t>لا يوجد حالياً أخبار جديدة عن البوابة</t>
+          <t>فرص التمويل قيد الدراسة</t>
         </is>
       </c>
       <c r="B531" t="inlineStr"/>
@@ -4683,7 +4683,7 @@
     <row r="532">
       <c r="A532" t="inlineStr">
         <is>
-          <t>عودة إلى الصفحة الرئيسية</t>
+          <t>لا يوجد حالياً فرص فرص تمويل للموافقة على النشر</t>
         </is>
       </c>
       <c r="B532" t="inlineStr"/>
@@ -4691,7 +4691,7 @@
     <row r="533">
       <c r="A533" t="inlineStr">
         <is>
-          <t>إضافة تقرير</t>
+          <t>اضافة فرصة تمويل</t>
         </is>
       </c>
       <c r="B533" t="inlineStr"/>
@@ -4699,7 +4699,7 @@
     <row r="534">
       <c r="A534" t="inlineStr">
         <is>
-          <t>حذف التقرير</t>
+          <t>اضافة</t>
         </is>
       </c>
       <c r="B534" t="inlineStr"/>
@@ -4707,7 +4707,7 @@
     <row r="535">
       <c r="A535" t="inlineStr">
         <is>
-          <t>هل أنت متأكد من رغبتك في حذف التقرير بعنوان</t>
+          <t>تعديل فرصة التمويل</t>
         </is>
       </c>
       <c r="B535" t="inlineStr"/>
@@ -4715,7 +4715,7 @@
     <row r="536">
       <c r="A536" t="inlineStr">
         <is>
-          <t>تفاصيل التقرير أو الدراسة</t>
+          <t>لا يوجد حالياً فرص تمويل منشورة من قبل المنظمات</t>
         </is>
       </c>
       <c r="B536" t="inlineStr"/>
@@ -4723,7 +4723,7 @@
     <row r="537">
       <c r="A537" t="inlineStr">
         <is>
-          <t>اسم اللذي أضاف التقرير</t>
+          <t>حذف فرصة التمويل</t>
         </is>
       </c>
       <c r="B537" t="inlineStr"/>
@@ -4731,7 +4731,7 @@
     <row r="538">
       <c r="A538" t="inlineStr">
         <is>
-          <t>تاريخ إضافة التقرير</t>
+          <t>هل أنت متأكد من رغبتك في حذف فرصة التمويل بعنوان</t>
         </is>
       </c>
       <c r="B538" t="inlineStr"/>
@@ -4739,7 +4739,7 @@
     <row r="539">
       <c r="A539" t="inlineStr">
         <is>
-          <t>محتوى التقرير</t>
+          <t>تفاصيل فرصة التمويل</t>
         </is>
       </c>
       <c r="B539" t="inlineStr"/>
@@ -4747,7 +4747,7 @@
     <row r="540">
       <c r="A540" t="inlineStr">
         <is>
-          <t>الموافقة على نشر التقرير</t>
+          <t>اسم اللذي أضاف فرصة التمويل</t>
         </is>
       </c>
       <c r="B540" t="inlineStr"/>
@@ -4755,7 +4755,7 @@
     <row r="541">
       <c r="A541" t="inlineStr">
         <is>
-          <t>إلغاء نشر التقرير</t>
+          <t>أحدث فرص تمويل المنظمات</t>
         </is>
       </c>
       <c r="B541" t="inlineStr"/>
@@ -4763,7 +4763,7 @@
     <row r="542">
       <c r="A542" t="inlineStr">
         <is>
-          <t>تعديل التقرير</t>
+          <t>الموافقة على النشر</t>
         </is>
       </c>
       <c r="B542" t="inlineStr"/>
@@ -4771,7 +4771,7 @@
     <row r="543">
       <c r="A543" t="inlineStr">
         <is>
-          <t>التقارير و الدراسات</t>
+          <t>إلغاء نشر فرصة التمويل</t>
         </is>
       </c>
       <c r="B543" t="inlineStr"/>
@@ -4779,7 +4779,7 @@
     <row r="544">
       <c r="A544" t="inlineStr">
         <is>
-          <t>إضافة تقرير أو دراسة</t>
+          <t>إضافة فرصة تمويل للأفراد</t>
         </is>
       </c>
       <c r="B544" t="inlineStr"/>
@@ -4787,7 +4787,7 @@
     <row r="545">
       <c r="A545" t="inlineStr">
         <is>
-          <t>لقراءة ملف الدراسة يجب الدخول إلى التفاصيل</t>
+          <t>حذف فرصة تمويل للأفراد</t>
         </is>
       </c>
       <c r="B545" t="inlineStr"/>
@@ -4795,7 +4795,7 @@
     <row r="546">
       <c r="A546" t="inlineStr">
         <is>
-          <t>لا يوجد حالياً تقارير و دراسات للموافقة على النشر</t>
+          <t>تفاصيل فرصة تمويل للأفراد</t>
         </is>
       </c>
       <c r="B546" t="inlineStr"/>
@@ -4803,7 +4803,7 @@
     <row r="547">
       <c r="A547" t="inlineStr">
         <is>
-          <t>إضافة بحث</t>
+          <t>تعديل فرصة تمويل للأفراد</t>
         </is>
       </c>
       <c r="B547" t="inlineStr"/>
@@ -4811,7 +4811,7 @@
     <row r="548">
       <c r="A548" t="inlineStr">
         <is>
-          <t>حذف البحث الخارجي</t>
+          <t>فرص التمويل للأفراد للموافقة على النشر</t>
         </is>
       </c>
       <c r="B548" t="inlineStr"/>
@@ -4819,7 +4819,7 @@
     <row r="549">
       <c r="A549" t="inlineStr">
         <is>
-          <t>هل أنت متأكد من رغبتك في حذف البحث بعنوان</t>
+          <t>لا يوجد حالياً فرص للأفراد تمويل منشورة من قبل المنظمات</t>
         </is>
       </c>
       <c r="B549" t="inlineStr"/>
@@ -4827,7 +4827,7 @@
     <row r="550">
       <c r="A550" t="inlineStr">
         <is>
-          <t>حذف البحث</t>
+          <t>فرص التمويل للأفراد</t>
         </is>
       </c>
       <c r="B550" t="inlineStr"/>
@@ -4835,7 +4835,7 @@
     <row r="551">
       <c r="A551" t="inlineStr">
         <is>
-          <t>تفاصيل البحث الخارجي</t>
+          <t>قائمة دليل المجتمع المدني للموافقة على النشر</t>
         </is>
       </c>
       <c r="B551" t="inlineStr"/>
@@ -4843,7 +4843,7 @@
     <row r="552">
       <c r="A552" t="inlineStr">
         <is>
-          <t>اسم اللذي أضاف البحث</t>
+          <t>للمزيد عن المنظمة</t>
         </is>
       </c>
       <c r="B552" t="inlineStr"/>
@@ -4851,7 +4851,7 @@
     <row r="553">
       <c r="A553" t="inlineStr">
         <is>
-          <t>تاريخ إضافة البحث</t>
+          <t>حالياً لا يوجد طلبات للمنظمات للموافقة عليها</t>
         </is>
       </c>
       <c r="B553" t="inlineStr"/>
@@ -4859,7 +4859,7 @@
     <row r="554">
       <c r="A554" t="inlineStr">
         <is>
-          <t>محتوى البحث</t>
+          <t>عودة إلى صفحة دليل المنظمات</t>
         </is>
       </c>
       <c r="B554" t="inlineStr"/>
@@ -4867,7 +4867,7 @@
     <row r="555">
       <c r="A555" t="inlineStr">
         <is>
-          <t>الموافقة على نشر البحث</t>
+          <t>إقراء المزيد</t>
         </is>
       </c>
       <c r="B555" t="inlineStr"/>
@@ -4875,7 +4875,7 @@
     <row r="556">
       <c r="A556" t="inlineStr">
         <is>
-          <t>إلغاء نشر البحث</t>
+          <t>قائمة منظمات المجتمع المدني</t>
         </is>
       </c>
       <c r="B556" t="inlineStr"/>
@@ -4883,7 +4883,7 @@
     <row r="557">
       <c r="A557" t="inlineStr">
         <is>
-          <t>تعديل البحث</t>
+          <t>طلبات اشتراك المنظمات قيد الدراسة</t>
         </is>
       </c>
       <c r="B557" t="inlineStr"/>
@@ -4891,7 +4891,7 @@
     <row r="558">
       <c r="A558" t="inlineStr">
         <is>
-          <t>اﻷبحاث الخارجية</t>
+          <t>إجمالي عدد المنظمات</t>
         </is>
       </c>
       <c r="B558" t="inlineStr"/>
@@ -4899,7 +4899,7 @@
     <row r="559">
       <c r="A559" t="inlineStr">
         <is>
-          <t>إضافة بحث خارجي</t>
+          <t>حالياً لا يوجد منظمات مسجله او موافق عليها</t>
         </is>
       </c>
       <c r="B559" t="inlineStr"/>
@@ -4907,7 +4907,7 @@
     <row r="560">
       <c r="A560" t="inlineStr">
         <is>
-          <t>لا يوجد حالياً أبحاث خارجية منشورة للمنظمات</t>
+          <t>دليل المجتمع المدني بحسب مجال العمل</t>
         </is>
       </c>
       <c r="B560" t="inlineStr"/>
@@ -4915,7 +4915,7 @@
     <row r="561">
       <c r="A561" t="inlineStr">
         <is>
-          <t>اﻷبحاث الخارجية قيد الدراسة</t>
+          <t>المنظمات المضافة حديثاً</t>
         </is>
       </c>
       <c r="B561" t="inlineStr"/>
@@ -4923,7 +4923,7 @@
     <row r="562">
       <c r="A562" t="inlineStr">
         <is>
-          <t>لا يوجد حالياً أبحاث خارجية قيد الدراسة</t>
+          <t>أحدث اﻷخبار</t>
         </is>
       </c>
       <c r="B562" t="inlineStr"/>
@@ -4931,7 +4931,7 @@
     <row r="563">
       <c r="A563" t="inlineStr">
         <is>
-          <t>فرص العمل قيد الدراسة</t>
+          <t>للمزيد عن الخبر</t>
         </is>
       </c>
       <c r="B563" t="inlineStr"/>
@@ -4939,7 +4939,7 @@
     <row r="564">
       <c r="A564" t="inlineStr">
         <is>
-          <t>لا يوجد حالياً فرص عمل للموافقة على النشر</t>
+          <t>أحدث فرص العمل</t>
         </is>
       </c>
       <c r="B564" t="inlineStr"/>
@@ -4947,7 +4947,7 @@
     <row r="565">
       <c r="A565" t="inlineStr">
         <is>
-          <t>انشر فرصة العمل</t>
+          <t>للمزيد عن فرصة العمل</t>
         </is>
       </c>
       <c r="B565" t="inlineStr"/>
@@ -4955,7 +4955,7 @@
     <row r="566">
       <c r="A566" t="inlineStr">
         <is>
-          <t>تعديل فرصة عمل</t>
+          <t>أحدث فرص بناء القدرات</t>
         </is>
       </c>
       <c r="B566" t="inlineStr"/>
@@ -4963,7 +4963,7 @@
     <row r="567">
       <c r="A567" t="inlineStr">
         <is>
-          <t>حذف فرصة عمل</t>
+          <t>للمزيد عن فرصة بناء القدرات</t>
         </is>
       </c>
       <c r="B567" t="inlineStr"/>
@@ -4971,7 +4971,7 @@
     <row r="568">
       <c r="A568" t="inlineStr">
         <is>
-          <t xml:space="preserve">هل أنت متأكد من رغبتك في حذف فرصة العمل بعنوان </t>
+          <t>اشترك</t>
         </is>
       </c>
       <c r="B568" t="inlineStr"/>
@@ -4979,7 +4979,7 @@
     <row r="569">
       <c r="A569" t="inlineStr">
         <is>
-          <t>تفاصيل العمل</t>
+          <t>إضافة محتوى سمعي و بصري</t>
         </is>
       </c>
       <c r="B569" t="inlineStr"/>
@@ -4987,7 +4987,7 @@
     <row r="570">
       <c r="A570" t="inlineStr">
         <is>
-          <t xml:space="preserve"> تفاصيل العمل</t>
+          <t>إضافة</t>
         </is>
       </c>
       <c r="B570" t="inlineStr"/>
@@ -4995,7 +4995,7 @@
     <row r="571">
       <c r="A571" t="inlineStr">
         <is>
-          <t>اسم اللذي أضاف فرصة العمل</t>
+          <t>حذف المحتوى السمعي و البصري</t>
         </is>
       </c>
       <c r="B571" t="inlineStr"/>
@@ -5003,7 +5003,7 @@
     <row r="572">
       <c r="A572" t="inlineStr">
         <is>
-          <t>عنوان فرصة العمل</t>
+          <t>هل أنت متأكد من رغبتك في حذف المحتوى بعنوان</t>
         </is>
       </c>
       <c r="B572" t="inlineStr"/>
@@ -5011,7 +5011,7 @@
     <row r="573">
       <c r="A573" t="inlineStr">
         <is>
-          <t>وصف فرصة العمل</t>
+          <t>حذف المحتوى</t>
         </is>
       </c>
       <c r="B573" t="inlineStr"/>
@@ -5019,7 +5019,7 @@
     <row r="574">
       <c r="A574" t="inlineStr">
         <is>
-          <t>إلغاء نشر فرصة العمل</t>
+          <t>تعديل المحتوى السمعي و البصري</t>
         </is>
       </c>
       <c r="B574" t="inlineStr"/>
@@ -5027,7 +5027,7 @@
     <row r="575">
       <c r="A575" t="inlineStr">
         <is>
-          <t>لا يوجد حالياً فرص عمل</t>
+          <t>المحتوى السمعي و البصري</t>
         </is>
       </c>
       <c r="B575" t="inlineStr"/>
@@ -5035,7 +5035,7 @@
     <row r="576">
       <c r="A576" t="inlineStr">
         <is>
-          <t>مصادر المجتمع المدني</t>
+          <t xml:space="preserve"> لا يوجد حالياً محتوى سمعي و بصري منشور من قبل المنظمات</t>
         </is>
       </c>
       <c r="B576" t="inlineStr"/>
@@ -5043,7 +5043,7 @@
     <row r="577">
       <c r="A577" t="inlineStr">
         <is>
-          <t>المصادر</t>
+          <t>تفاصيل المحتوى السمعي والبصري</t>
         </is>
       </c>
       <c r="B577" t="inlineStr"/>
@@ -5051,7 +5051,7 @@
     <row r="578">
       <c r="A578" t="inlineStr">
         <is>
-          <t>تعديل ملفي الشخصي</t>
+          <t>اسم اللذي أضاف المحتوى</t>
         </is>
       </c>
       <c r="B578" t="inlineStr"/>
@@ -5059,7 +5059,7 @@
     <row r="579">
       <c r="A579" t="inlineStr">
         <is>
-          <t>حذف الملف</t>
+          <t>تاريخ إضافة المحتوى</t>
         </is>
       </c>
       <c r="B579" t="inlineStr"/>
@@ -5067,7 +5067,7 @@
     <row r="580">
       <c r="A580" t="inlineStr">
         <is>
-          <t>هل أنت متأكد من رغبتك في حذف الملف الشخصي</t>
+          <t>مضمون المحتوى السمعي و البصري</t>
         </is>
       </c>
       <c r="B580" t="inlineStr"/>
@@ -5075,7 +5075,7 @@
     <row r="581">
       <c r="A581" t="inlineStr">
         <is>
-          <t>لا يوجد لديك الصلاحية للدخول إلى هذه الصفحة</t>
+          <t>الموافقة على نشر المحتوى</t>
         </is>
       </c>
       <c r="B581" t="inlineStr"/>
@@ -5083,7 +5083,7 @@
     <row r="582">
       <c r="A582" t="inlineStr">
         <is>
-          <t>اتمام الملف الشخصي للمنظمة</t>
+          <t>إلغاء نشر المحتوى</t>
         </is>
       </c>
       <c r="B582" t="inlineStr"/>
@@ -5091,7 +5091,7 @@
     <row r="583">
       <c r="A583" t="inlineStr">
         <is>
-          <t>تقديم طلب اشتراك</t>
+          <t>تعديل المحتوى</t>
         </is>
       </c>
       <c r="B583" t="inlineStr"/>
@@ -5099,7 +5099,7 @@
     <row r="584">
       <c r="A584" t="inlineStr">
         <is>
-          <t>هذا الحقل لا يقبل أقل من 3 حروف و لا يقبل اﻷحرف الخاصه و الرموز</t>
+          <t>المحتوى السمعي و البصري قيد الدراسة</t>
         </is>
       </c>
       <c r="B584" t="inlineStr"/>
@@ -5107,7 +5107,7 @@
     <row r="585">
       <c r="A585" t="inlineStr">
         <is>
-          <t>تعديل الملف الشخصي للمنظمة</t>
+          <t>لا يوجد حالياً محتوى سمعي و بصري منشور من قبل المنظمات للموافقة على النشر</t>
         </is>
       </c>
       <c r="B585" t="inlineStr"/>
@@ -5115,7 +5115,7 @@
     <row r="586">
       <c r="A586" t="inlineStr">
         <is>
-          <t>حالياً لا يوجد منظمات مسجله او للموافقة عليها</t>
+          <t>انشر الخبر</t>
         </is>
       </c>
       <c r="B586" t="inlineStr"/>
@@ -5123,7 +5123,7 @@
     <row r="587">
       <c r="A587" t="inlineStr">
         <is>
-          <t>تفاصيل المنظمة</t>
+          <t>تعديل خبر</t>
         </is>
       </c>
       <c r="B587" t="inlineStr"/>
@@ -5131,7 +5131,7 @@
     <row r="588">
       <c r="A588" t="inlineStr">
         <is>
-          <t>لم يذكر</t>
+          <t>تعديل الخبر</t>
         </is>
       </c>
       <c r="B588" t="inlineStr"/>
@@ -5139,7 +5139,7 @@
     <row r="589">
       <c r="A589" t="inlineStr">
         <is>
-          <t>اسم الذي أضاف المنظمة</t>
+          <t>حذف خبر</t>
         </is>
       </c>
       <c r="B589" t="inlineStr"/>
@@ -5147,7 +5147,7 @@
     <row r="590">
       <c r="A590" t="inlineStr">
         <is>
-          <t>عن المنظمة</t>
+          <t xml:space="preserve">هل أنت متأكد من رغبتك في حذف الخبر بعنوان </t>
         </is>
       </c>
       <c r="B590" t="inlineStr"/>
@@ -5155,7 +5155,7 @@
     <row r="591">
       <c r="A591" t="inlineStr">
         <is>
-          <t>معلومات الاتصال بالمنظمة</t>
+          <t>حذف الخبر</t>
         </is>
       </c>
       <c r="B591" t="inlineStr"/>
@@ -5163,7 +5163,7 @@
     <row r="592">
       <c r="A592" t="inlineStr">
         <is>
-          <t>جديد المنظمة</t>
+          <t>لا يوجد حالياً أخبار للموافقة على النشر</t>
         </is>
       </c>
       <c r="B592" t="inlineStr"/>
@@ -5171,7 +5171,7 @@
     <row r="593">
       <c r="A593" t="inlineStr">
         <is>
-          <t>معلومات عن المنظمة</t>
+          <t>تاريخ إضافة الخبر</t>
         </is>
       </c>
       <c r="B593" t="inlineStr"/>
@@ -5179,7 +5179,7 @@
     <row r="594">
       <c r="A594" t="inlineStr">
         <is>
-          <t>نعم مسجلة</t>
+          <t>اسم اللذي أضاف الخبر</t>
         </is>
       </c>
       <c r="B594" t="inlineStr"/>
@@ -5187,7 +5187,7 @@
     <row r="595">
       <c r="A595" t="inlineStr">
         <is>
-          <t>غير مسجلة</t>
+          <t>أحدث ثلاثة أخبار</t>
         </is>
       </c>
       <c r="B595" t="inlineStr"/>
@@ -5195,7 +5195,7 @@
     <row r="596">
       <c r="A596" t="inlineStr">
         <is>
-          <t>ليست عضو</t>
+          <t>الموافقة على نشر الخبر</t>
         </is>
       </c>
       <c r="B596" t="inlineStr"/>
@@ -5203,7 +5203,7 @@
     <row r="597">
       <c r="A597" t="inlineStr">
         <is>
-          <t>اسم الشبكة أو التحالف</t>
+          <t>لا يوجد حالياً أخبار منشورة للمنظمات</t>
         </is>
       </c>
       <c r="B597" t="inlineStr"/>
@@ -5211,7 +5211,7 @@
     <row r="598">
       <c r="A598" t="inlineStr">
         <is>
-          <t>هل تم التحقق من قبل اﻹدارة على أنها منظمة؟</t>
+          <t>اخبار البوابة</t>
         </is>
       </c>
       <c r="B598" t="inlineStr"/>
@@ -5219,7 +5219,7 @@
     <row r="599">
       <c r="A599" t="inlineStr">
         <is>
-          <t>تم التحقق و الموافقة</t>
+          <t xml:space="preserve">اخبار البوابة </t>
         </is>
       </c>
       <c r="B599" t="inlineStr"/>
@@ -5227,7 +5227,7 @@
     <row r="600">
       <c r="A600" t="inlineStr">
         <is>
-          <t>لم يتم التحقق بعد</t>
+          <t>أخبار البوابةقيد الدراسة</t>
         </is>
       </c>
       <c r="B600" t="inlineStr"/>
@@ -5235,7 +5235,7 @@
     <row r="601">
       <c r="A601" t="inlineStr">
         <is>
-          <t>أخبار المنظمة</t>
+          <t>لا يوجد حالياً أخبار جديدة عن البوابة</t>
         </is>
       </c>
       <c r="B601" t="inlineStr"/>
@@ -5243,7 +5243,7 @@
     <row r="602">
       <c r="A602" t="inlineStr">
         <is>
-          <t>التقارير و الدراسات للمنظمة</t>
+          <t>عودة إلى الصفحة الرئيسية</t>
         </is>
       </c>
       <c r="B602" t="inlineStr"/>
@@ -5251,7 +5251,7 @@
     <row r="603">
       <c r="A603" t="inlineStr">
         <is>
-          <t>البيانات للمنظمة</t>
+          <t>إضافة تقرير</t>
         </is>
       </c>
       <c r="B603" t="inlineStr"/>
@@ -5259,7 +5259,7 @@
     <row r="604">
       <c r="A604" t="inlineStr">
         <is>
-          <t>المحتوى السمعي و البصري للمنظمة</t>
+          <t>حذف التقرير</t>
         </is>
       </c>
       <c r="B604" t="inlineStr"/>
@@ -5267,7 +5267,7 @@
     <row r="605">
       <c r="A605" t="inlineStr">
         <is>
-          <t>قبول الطلب</t>
+          <t>هل أنت متأكد من رغبتك في حذف التقرير بعنوان</t>
         </is>
       </c>
       <c r="B605" t="inlineStr"/>
@@ -5275,7 +5275,7 @@
     <row r="606">
       <c r="A606" t="inlineStr">
         <is>
-          <t>رفض الطلب</t>
+          <t>تفاصيل التقرير أو الدراسة</t>
         </is>
       </c>
       <c r="B606" t="inlineStr"/>
@@ -5283,7 +5283,7 @@
     <row r="607">
       <c r="A607" t="inlineStr">
         <is>
-          <t>حذف الطلب</t>
+          <t>اسم اللذي أضاف التقرير</t>
         </is>
       </c>
       <c r="B607" t="inlineStr"/>
@@ -5291,7 +5291,7 @@
     <row r="608">
       <c r="A608" t="inlineStr">
         <is>
-          <t>تعديل الملف الشخصي</t>
+          <t>تاريخ إضافة التقرير</t>
         </is>
       </c>
       <c r="B608" t="inlineStr"/>
@@ -5299,7 +5299,7 @@
     <row r="609">
       <c r="A609" t="inlineStr">
         <is>
-          <t>حذف الملف الشخصي</t>
+          <t>محتوى التقرير</t>
         </is>
       </c>
       <c r="B609" t="inlineStr"/>
@@ -5307,7 +5307,7 @@
     <row r="610">
       <c r="A610" t="inlineStr">
         <is>
-          <t>عودة إلى صفحة دليل المجتمع المدني</t>
+          <t>الموافقة على نشر التقرير</t>
         </is>
       </c>
       <c r="B610" t="inlineStr"/>
@@ -5315,7 +5315,7 @@
     <row r="611">
       <c r="A611" t="inlineStr">
         <is>
-          <t>الملف الشخصي</t>
+          <t>إلغاء نشر التقرير</t>
         </is>
       </c>
       <c r="B611" t="inlineStr"/>
@@ -5323,7 +5323,7 @@
     <row r="612">
       <c r="A612" t="inlineStr">
         <is>
-          <t>اسم المنظمة المختصر</t>
+          <t>تعديل التقرير</t>
         </is>
       </c>
       <c r="B612" t="inlineStr"/>
@@ -5331,7 +5331,7 @@
     <row r="613">
       <c r="A613" t="inlineStr">
         <is>
-          <t>التأكيد من اﻹدارة على أنها منظمة</t>
+          <t>التقارير و الدراسات</t>
         </is>
       </c>
       <c r="B613" t="inlineStr"/>
@@ -5339,7 +5339,7 @@
     <row r="614">
       <c r="A614" t="inlineStr">
         <is>
-          <t>تمت الموافقة عليها</t>
+          <t>إضافة تقرير أو دراسة</t>
         </is>
       </c>
       <c r="B614" t="inlineStr"/>
@@ -5347,7 +5347,7 @@
     <row r="615">
       <c r="A615" t="inlineStr">
         <is>
-          <t>لم يتم التأكيد بعد</t>
+          <t>لقراءة ملف الدراسة يجب الدخول إلى التفاصيل</t>
         </is>
       </c>
       <c r="B615" t="inlineStr"/>
@@ -5355,7 +5355,7 @@
     <row r="616">
       <c r="A616" t="inlineStr">
         <is>
-          <t>تعديل الطلب</t>
+          <t>لا يوجد حالياً تقارير و دراسات للموافقة على النشر</t>
         </is>
       </c>
       <c r="B616" t="inlineStr"/>
@@ -5363,7 +5363,7 @@
     <row r="617">
       <c r="A617" t="inlineStr">
         <is>
-          <t>رجاءً أتمم ملف المنظمة الشخصي لنتمكن من التحقق من معلوماتكم و تتمكنون من استخدام الموقع</t>
+          <t>إضافة بحث</t>
         </is>
       </c>
       <c r="B617" t="inlineStr"/>
@@ -5371,7 +5371,7 @@
     <row r="618">
       <c r="A618" t="inlineStr">
         <is>
-          <t>ملف المنظمة الشخصي</t>
+          <t>حذف البحث الخارجي</t>
         </is>
       </c>
       <c r="B618" t="inlineStr"/>
@@ -5379,7 +5379,7 @@
     <row r="619">
       <c r="A619" t="inlineStr">
         <is>
-          <t>تقديم طلب اشتراك لمنظمة</t>
+          <t>هل أنت متأكد من رغبتك في حذف البحث بعنوان</t>
         </is>
       </c>
       <c r="B619" t="inlineStr"/>
@@ -5387,7 +5387,7 @@
     <row r="620">
       <c r="A620" t="inlineStr">
         <is>
-          <t>تنشيط الحساب</t>
+          <t>حذف البحث</t>
         </is>
       </c>
       <c r="B620" t="inlineStr"/>
@@ -5395,7 +5395,7 @@
     <row r="621">
       <c r="A621" t="inlineStr">
         <is>
-          <t>لقد تم تسجيل الخروج بنجاح</t>
+          <t>تفاصيل البحث الخارجي</t>
         </is>
       </c>
       <c r="B621" t="inlineStr"/>
@@ -5403,7 +5403,7 @@
     <row r="622">
       <c r="A622" t="inlineStr">
         <is>
-          <t>يمكنك اﻵن</t>
+          <t>اسم اللذي أضاف البحث</t>
         </is>
       </c>
       <c r="B622" t="inlineStr"/>
@@ -5411,7 +5411,7 @@
     <row r="623">
       <c r="A623" t="inlineStr">
         <is>
-          <t>إعادة تسجيل الدخول</t>
+          <t>تاريخ إضافة البحث</t>
         </is>
       </c>
       <c r="B623" t="inlineStr"/>
@@ -5419,7 +5419,7 @@
     <row r="624">
       <c r="A624" t="inlineStr">
         <is>
-          <t>الذهاب للصفحة الرئيسية</t>
+          <t>محتوى البحث</t>
         </is>
       </c>
       <c r="B624" t="inlineStr"/>
@@ -5427,7 +5427,7 @@
     <row r="625">
       <c r="A625" t="inlineStr">
         <is>
-          <t>تغيير</t>
+          <t>الموافقة على نشر البحث</t>
         </is>
       </c>
       <c r="B625" t="inlineStr"/>
@@ -5435,7 +5435,7 @@
     <row r="626">
       <c r="A626" t="inlineStr">
         <is>
-          <t>لقد تم تغيير كلمة المرور بنجاح</t>
+          <t>إلغاء نشر البحث</t>
         </is>
       </c>
       <c r="B626" t="inlineStr"/>
@@ -5443,7 +5443,7 @@
     <row r="627">
       <c r="A627" t="inlineStr">
         <is>
-          <t>يمكنك اﻵن تسجيل الدخول باستخدام كلمة المرور الجديدة</t>
+          <t>تعديل البحث</t>
         </is>
       </c>
       <c r="B627" t="inlineStr"/>
@@ -5451,7 +5451,7 @@
     <row r="628">
       <c r="A628" t="inlineStr">
         <is>
-          <t>إعادة تعيين كلمة المرور</t>
+          <t>اﻷبحاث الخارجية</t>
         </is>
       </c>
       <c r="B628" t="inlineStr"/>
@@ -5459,7 +5459,7 @@
     <row r="629">
       <c r="A629" t="inlineStr">
         <is>
-          <t>لا يمكنك إعادة تعيين كلمة المرور بحال تسجيل الدخول</t>
+          <t>إضافة بحث خارجي</t>
         </is>
       </c>
       <c r="B629" t="inlineStr"/>
@@ -5467,7 +5467,7 @@
     <row r="630">
       <c r="A630" t="inlineStr">
         <is>
-          <t>تغيير كلمة السر</t>
+          <t>لا يوجد حالياً أبحاث خارجية منشورة للمنظمات</t>
         </is>
       </c>
       <c r="B630" t="inlineStr"/>
@@ -5475,7 +5475,7 @@
     <row r="631">
       <c r="A631" t="inlineStr">
         <is>
-          <t>إعادة تعيين</t>
+          <t>اﻷبحاث الخارجية قيد الدراسة</t>
         </is>
       </c>
       <c r="B631" t="inlineStr"/>
@@ -5483,7 +5483,7 @@
     <row r="632">
       <c r="A632" t="inlineStr">
         <is>
-          <t>لقد تم إعادة تعيين كلمة المرور بنجاح</t>
+          <t>لا يوجد حالياً أبحاث خارجية قيد الدراسة</t>
         </is>
       </c>
       <c r="B632" t="inlineStr"/>
@@ -5491,7 +5491,7 @@
     <row r="633">
       <c r="A633" t="inlineStr">
         <is>
-          <t>يمكنك ﻵن</t>
+          <t>فرص العمل قيد الدراسة</t>
         </is>
       </c>
       <c r="B633" t="inlineStr"/>
@@ -5499,7 +5499,7 @@
     <row r="634">
       <c r="A634" t="inlineStr">
         <is>
-          <t>تسحيل الدخول</t>
+          <t>اسم العمل</t>
         </is>
       </c>
       <c r="B634" t="inlineStr"/>
@@ -5507,7 +5507,7 @@
     <row r="635">
       <c r="A635" t="inlineStr">
         <is>
-          <t>أو</t>
+          <t>مدة العمل</t>
         </is>
       </c>
       <c r="B635" t="inlineStr"/>
@@ -5515,7 +5515,7 @@
     <row r="636">
       <c r="A636" t="inlineStr">
         <is>
-          <t>الصفحة الرئيسية</t>
+          <t>أشهر</t>
         </is>
       </c>
       <c r="B636" t="inlineStr"/>
@@ -5523,7 +5523,7 @@
     <row r="637">
       <c r="A637" t="inlineStr">
         <is>
-          <t>تأكيد إعادة تعيين كلمة المرور</t>
+          <t>لا يوجد حالياً فرص عمل للموافقة على النشر</t>
         </is>
       </c>
       <c r="B637" t="inlineStr"/>
@@ -5531,7 +5531,7 @@
     <row r="638">
       <c r="A638" t="inlineStr">
         <is>
-          <t>يتم إعادة تعيين كلمة المرور</t>
+          <t>انشر فرصة العمل</t>
         </is>
       </c>
       <c r="B638" t="inlineStr"/>
@@ -5539,7 +5539,7 @@
     <row r="639">
       <c r="A639" t="inlineStr">
         <is>
-          <t>لقد تم إرسال بريد الكتروني يتضمن رابط ﻹعادة تعيين كلمة المرور</t>
+          <t>تعديل فرصة عمل</t>
         </is>
       </c>
       <c r="B639" t="inlineStr"/>
@@ -5547,7 +5547,7 @@
     <row r="640">
       <c r="A640" t="inlineStr">
         <is>
-          <t>يمكنك الذهاب إلى</t>
+          <t>حذف فرصة عمل</t>
         </is>
       </c>
       <c r="B640" t="inlineStr"/>
@@ -5555,7 +5555,7 @@
     <row r="641">
       <c r="A641" t="inlineStr">
         <is>
-          <t>هل نسيت كلمة المرور</t>
+          <t xml:space="preserve">هل أنت متأكد من رغبتك في حذف فرصة العمل بعنوان </t>
         </is>
       </c>
       <c r="B641" t="inlineStr"/>
@@ -5563,7 +5563,7 @@
     <row r="642">
       <c r="A642" t="inlineStr">
         <is>
-          <t>إذا لم يكن لديك حساب ! يمكنك</t>
+          <t>تفاصيل العمل</t>
         </is>
       </c>
       <c r="B642" t="inlineStr"/>
@@ -5571,7 +5571,7 @@
     <row r="643">
       <c r="A643" t="inlineStr">
         <is>
-          <t>إنشاء حساب</t>
+          <t xml:space="preserve"> تفاصيل العمل</t>
         </is>
       </c>
       <c r="B643" t="inlineStr"/>
@@ -5579,7 +5579,7 @@
     <row r="644">
       <c r="A644" t="inlineStr">
         <is>
-          <t>أنشاء حساب</t>
+          <t>اسم فرصة العمل</t>
         </is>
       </c>
       <c r="B644" t="inlineStr"/>
@@ -5587,7 +5587,7 @@
     <row r="645">
       <c r="A645" t="inlineStr">
         <is>
-          <t>تقديم طلب اشترك</t>
+          <t>اسم اللذي أضاف فرصة العمل</t>
         </is>
       </c>
       <c r="B645" t="inlineStr"/>
@@ -5595,10 +5595,602 @@
     <row r="646">
       <c r="A646" t="inlineStr">
         <is>
+          <t>وصف فرصة العمل</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr"/>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>المدينة</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr"/>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>الخبرة المطلوبة</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr"/>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>تاريخ إغلاق التقدم للوظيفة</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr"/>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>إلغاء نشر فرصة العمل</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr"/>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>لا يوجد حالياً فرص عمل</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr"/>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>مصادر المجتمع المدني</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr"/>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>المصادر</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr"/>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>تعديل ملفي الشخصي</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr"/>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>حذف الملف</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr"/>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>هل أنت متأكد من رغبتك في حذف الملف الشخصي</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr"/>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>لا يوجد لديك الصلاحية للدخول إلى هذه الصفحة</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr"/>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>اتمام الملف الشخصي للمنظمة</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr"/>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>تقديم طلب اشتراك</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr"/>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>هذا الحقل لا يقبل أقل من 3 حروف و لا يقبل اﻷحرف الخاصه و الرموز</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr"/>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>تعديل الملف الشخصي للمنظمة</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr"/>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>حالياً لا يوجد منظمات مسجله او للموافقة عليها</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr"/>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>تفاصيل المنظمة</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr"/>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>عن المنظمة</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr"/>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>معلومات الاتصال بالمنظمة</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr"/>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>جديد المنظمة</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr"/>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>معلومات عن المنظمة</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr"/>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>نعم مسجلة</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr"/>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>غير مسجلة</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr"/>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>ليست عضو</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr"/>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>اسم الشبكة أو التحالف</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr"/>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>هل تم التحقق من قبل اﻹدارة على أنها منظمة؟</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr"/>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>تم التحقق و الموافقة</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr"/>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>لم يتم التحقق بعد</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr"/>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>أخبار المنظمة</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr"/>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>التقارير و الدراسات للمنظمة</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr"/>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>البيانات للمنظمة</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr"/>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>المحتوى السمعي و البصري للمنظمة</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr"/>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>قبول الطلب</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr"/>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>رفض الطلب</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr"/>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>حذف الطلب</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr"/>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>تعديل الملف الشخصي</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr"/>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>حذف الملف الشخصي</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr"/>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>عودة إلى صفحة دليل المجتمع المدني</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr"/>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>الملف الشخصي</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr"/>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>اسم المنظمة المختصر</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr"/>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>التأكيد من اﻹدارة على أنها منظمة</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr"/>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>تمت الموافقة عليها</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr"/>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>لم يتم التأكيد بعد</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr"/>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>تعديل الطلب</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr"/>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>رجاءً أتمم ملف المنظمة الشخصي لنتمكن من التحقق من معلوماتكم و تتمكنون من استخدام الموقع</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr"/>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>ملف المنظمة الشخصي</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr"/>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>تقديم طلب اشتراك لمنظمة</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr"/>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>تنشيط الحساب</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr"/>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>لقد تم تسجيل الخروج بنجاح</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr"/>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>يمكنك اﻵن</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr"/>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>إعادة تسجيل الدخول</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr"/>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>الذهاب للصفحة الرئيسية</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr"/>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>تغيير</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr"/>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>لقد تم تغيير كلمة المرور بنجاح</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr"/>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>يمكنك اﻵن تسجيل الدخول باستخدام كلمة المرور الجديدة</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr"/>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>إعادة تعيين كلمة المرور</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr"/>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>لا يمكنك إعادة تعيين كلمة المرور بحال تسجيل الدخول</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr"/>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>تغيير كلمة السر</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr"/>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>إعادة تعيين</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr"/>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>لقد تم إعادة تعيين كلمة المرور بنجاح</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr"/>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>يمكنك ﻵن</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr"/>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>تسحيل الدخول</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr"/>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>أو</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr"/>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>الصفحة الرئيسية</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr"/>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>تأكيد إعادة تعيين كلمة المرور</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr"/>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>يتم إعادة تعيين كلمة المرور</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr"/>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>لقد تم إرسال بريد الكتروني يتضمن رابط ﻹعادة تعيين كلمة المرور</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr"/>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>يمكنك الذهاب إلى</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr"/>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>هل نسيت كلمة المرور</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr"/>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>إذا لم يكن لديك حساب ! يمكنك</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr"/>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>إنشاء حساب</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr"/>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>أنشاء حساب</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr"/>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>تقديم طلب اشترك</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr"/>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
           <t>إذا كان لديك حساب يمكنك تسجيل الدخول من هنا</t>
         </is>
       </c>
-      <c r="B646" t="inlineStr"/>
+      <c r="B720" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>